<commit_message>
Add ostrich and vulture nest
</commit_message>
<xml_diff>
--- a/form.xlsx
+++ b/form.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\aerialsurvey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83EB2B7A-B65D-43F8-99D7-898A7DD9A163}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54016476-EFBE-47B3-B144-524BCA9ED9CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="38220" windowHeight="15930" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11205" yWindow="1545" windowWidth="35190" windowHeight="12690" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="483">
   <si>
     <t>type</t>
   </si>
@@ -1447,6 +1447,30 @@
   </si>
   <si>
     <t>Birds.svg</t>
+  </si>
+  <si>
+    <t>Aaron Nicholas</t>
+  </si>
+  <si>
+    <t>aaron_nicholas</t>
+  </si>
+  <si>
+    <t>vulture_nest</t>
+  </si>
+  <si>
+    <t>ostrich_nest</t>
+  </si>
+  <si>
+    <t>Vulture nest</t>
+  </si>
+  <si>
+    <t>Ostrich nest</t>
+  </si>
+  <si>
+    <t>Vulture nest.svg</t>
+  </si>
+  <si>
+    <t>Ostrich nest.svg</t>
   </si>
 </sst>
 </file>
@@ -2236,10 +2260,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E137"/>
+  <dimension ref="A1:E140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A117" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A125" sqref="A125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2327,21 +2351,21 @@
         <v>73</v>
       </c>
       <c r="B7" t="s">
+        <v>476</v>
+      </c>
+      <c r="C7" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" t="s">
         <v>336</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>337</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" t="s">
-        <v>84</v>
-      </c>
-      <c r="C9" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2349,10 +2373,10 @@
         <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -2360,10 +2384,10 @@
         <v>43</v>
       </c>
       <c r="B11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2371,21 +2395,21 @@
         <v>43</v>
       </c>
       <c r="B12" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" t="s">
         <v>90</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>60</v>
-      </c>
-      <c r="B14" t="s">
-        <v>92</v>
-      </c>
-      <c r="C14" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -2393,21 +2417,21 @@
         <v>60</v>
       </c>
       <c r="B15" t="s">
+        <v>92</v>
+      </c>
+      <c r="C15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" t="s">
         <v>63</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>66</v>
-      </c>
-      <c r="B17" t="s">
-        <v>94</v>
-      </c>
-      <c r="C17" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2415,21 +2439,21 @@
         <v>66</v>
       </c>
       <c r="B18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" t="s">
         <v>96</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>97</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>69</v>
-      </c>
-      <c r="B20" t="s">
-        <v>98</v>
-      </c>
-      <c r="C20" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2437,10 +2461,10 @@
         <v>69</v>
       </c>
       <c r="B21" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C21" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -2448,24 +2472,21 @@
         <v>69</v>
       </c>
       <c r="B22" t="s">
+        <v>100</v>
+      </c>
+      <c r="C22" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" t="s">
         <v>102</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>103</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B24" t="s">
-        <v>104</v>
-      </c>
-      <c r="C24" t="s">
-        <v>105</v>
-      </c>
-      <c r="D24" t="s">
-        <v>472</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -2473,13 +2494,13 @@
         <v>50</v>
       </c>
       <c r="B25" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C25" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D25" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -2487,30 +2508,27 @@
         <v>50</v>
       </c>
       <c r="B26" t="s">
+        <v>106</v>
+      </c>
+      <c r="C26" t="s">
+        <v>107</v>
+      </c>
+      <c r="D26" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" t="s">
         <v>108</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>399</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D27" t="s">
         <v>473</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>56</v>
-      </c>
-      <c r="B28" t="s">
-        <v>441</v>
-      </c>
-      <c r="C28" t="s">
-        <v>442</v>
-      </c>
-      <c r="D28" t="s">
-        <v>391</v>
-      </c>
-      <c r="E28" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -2518,13 +2536,13 @@
         <v>56</v>
       </c>
       <c r="B29" t="s">
-        <v>188</v>
+        <v>441</v>
       </c>
       <c r="C29" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="D29" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E29" t="s">
         <v>104</v>
@@ -2535,13 +2553,13 @@
         <v>56</v>
       </c>
       <c r="B30" t="s">
-        <v>115</v>
+        <v>188</v>
       </c>
       <c r="C30" t="s">
-        <v>116</v>
+        <v>446</v>
       </c>
       <c r="D30" t="s">
-        <v>117</v>
+        <v>392</v>
       </c>
       <c r="E30" t="s">
         <v>104</v>
@@ -2552,13 +2570,13 @@
         <v>56</v>
       </c>
       <c r="B31" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="C31" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="D31" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="E31" t="s">
         <v>104</v>
@@ -2569,13 +2587,13 @@
         <v>56</v>
       </c>
       <c r="B32" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C32" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D32" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E32" t="s">
         <v>104</v>
@@ -2586,13 +2604,13 @@
         <v>56</v>
       </c>
       <c r="B33" t="s">
-        <v>178</v>
+        <v>112</v>
       </c>
       <c r="C33" t="s">
-        <v>179</v>
+        <v>113</v>
       </c>
       <c r="D33" t="s">
-        <v>180</v>
+        <v>114</v>
       </c>
       <c r="E33" t="s">
         <v>104</v>
@@ -2603,13 +2621,13 @@
         <v>56</v>
       </c>
       <c r="B34" t="s">
-        <v>118</v>
+        <v>178</v>
       </c>
       <c r="C34" t="s">
-        <v>119</v>
+        <v>179</v>
       </c>
       <c r="D34" t="s">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="E34" t="s">
         <v>104</v>
@@ -2620,13 +2638,13 @@
         <v>56</v>
       </c>
       <c r="B35" t="s">
-        <v>191</v>
+        <v>118</v>
       </c>
       <c r="C35" t="s">
-        <v>192</v>
+        <v>119</v>
       </c>
       <c r="D35" t="s">
-        <v>193</v>
+        <v>120</v>
       </c>
       <c r="E35" t="s">
         <v>104</v>
@@ -2637,13 +2655,13 @@
         <v>56</v>
       </c>
       <c r="B36" t="s">
-        <v>121</v>
+        <v>191</v>
       </c>
       <c r="C36" t="s">
-        <v>122</v>
+        <v>192</v>
       </c>
       <c r="D36" t="s">
-        <v>353</v>
+        <v>193</v>
       </c>
       <c r="E36" t="s">
         <v>104</v>
@@ -2654,13 +2672,13 @@
         <v>56</v>
       </c>
       <c r="B37" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C37" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D37" t="s">
-        <v>125</v>
+        <v>353</v>
       </c>
       <c r="E37" t="s">
         <v>104</v>
@@ -2671,13 +2689,13 @@
         <v>56</v>
       </c>
       <c r="B38" t="s">
-        <v>200</v>
+        <v>123</v>
       </c>
       <c r="C38" t="s">
-        <v>201</v>
+        <v>124</v>
       </c>
       <c r="D38" t="s">
-        <v>202</v>
+        <v>125</v>
       </c>
       <c r="E38" t="s">
         <v>104</v>
@@ -2688,13 +2706,13 @@
         <v>56</v>
       </c>
       <c r="B39" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="C39" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="D39" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="E39" t="s">
         <v>104</v>
@@ -2705,13 +2723,13 @@
         <v>56</v>
       </c>
       <c r="B40" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="C40" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="D40" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="E40" t="s">
         <v>104</v>
@@ -2722,13 +2740,13 @@
         <v>56</v>
       </c>
       <c r="B41" t="s">
-        <v>129</v>
+        <v>194</v>
       </c>
       <c r="C41" t="s">
-        <v>130</v>
+        <v>195</v>
       </c>
       <c r="D41" t="s">
-        <v>131</v>
+        <v>196</v>
       </c>
       <c r="E41" t="s">
         <v>104</v>
@@ -2739,13 +2757,13 @@
         <v>56</v>
       </c>
       <c r="B42" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="C42" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="D42" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="E42" t="s">
         <v>104</v>
@@ -2756,13 +2774,13 @@
         <v>56</v>
       </c>
       <c r="B43" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C43" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D43" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="E43" t="s">
         <v>104</v>
@@ -2773,13 +2791,13 @@
         <v>56</v>
       </c>
       <c r="B44" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C44" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D44" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E44" t="s">
         <v>104</v>
@@ -2790,13 +2808,13 @@
         <v>56</v>
       </c>
       <c r="B45" t="s">
-        <v>186</v>
+        <v>135</v>
       </c>
       <c r="C45" t="s">
-        <v>447</v>
+        <v>136</v>
       </c>
       <c r="D45" t="s">
-        <v>187</v>
+        <v>137</v>
       </c>
       <c r="E45" t="s">
         <v>104</v>
@@ -2807,13 +2825,13 @@
         <v>56</v>
       </c>
       <c r="B46" t="s">
-        <v>157</v>
+        <v>186</v>
       </c>
       <c r="C46" t="s">
-        <v>158</v>
+        <v>447</v>
       </c>
       <c r="D46" t="s">
-        <v>159</v>
+        <v>187</v>
       </c>
       <c r="E46" t="s">
         <v>104</v>
@@ -2824,13 +2842,13 @@
         <v>56</v>
       </c>
       <c r="B47" t="s">
-        <v>184</v>
+        <v>157</v>
       </c>
       <c r="C47" t="s">
-        <v>185</v>
+        <v>158</v>
       </c>
       <c r="D47" t="s">
-        <v>379</v>
+        <v>159</v>
       </c>
       <c r="E47" t="s">
         <v>104</v>
@@ -2841,13 +2859,13 @@
         <v>56</v>
       </c>
       <c r="B48" t="s">
-        <v>138</v>
+        <v>184</v>
       </c>
       <c r="C48" t="s">
-        <v>139</v>
+        <v>185</v>
       </c>
       <c r="D48" t="s">
-        <v>374</v>
+        <v>379</v>
       </c>
       <c r="E48" t="s">
         <v>104</v>
@@ -2858,13 +2876,13 @@
         <v>56</v>
       </c>
       <c r="B49" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C49" t="s">
-        <v>449</v>
+        <v>139</v>
       </c>
       <c r="D49" t="s">
-        <v>143</v>
+        <v>374</v>
       </c>
       <c r="E49" t="s">
         <v>104</v>
@@ -2875,13 +2893,13 @@
         <v>56</v>
       </c>
       <c r="B50" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C50" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="D50" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E50" t="s">
         <v>104</v>
@@ -2892,13 +2910,13 @@
         <v>56</v>
       </c>
       <c r="B51" t="s">
-        <v>181</v>
+        <v>140</v>
       </c>
       <c r="C51" t="s">
-        <v>182</v>
+        <v>448</v>
       </c>
       <c r="D51" t="s">
-        <v>183</v>
+        <v>141</v>
       </c>
       <c r="E51" t="s">
         <v>104</v>
@@ -2909,13 +2927,13 @@
         <v>56</v>
       </c>
       <c r="B52" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="C52" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="D52" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="E52" t="s">
         <v>104</v>
@@ -2926,13 +2944,13 @@
         <v>56</v>
       </c>
       <c r="B53" t="s">
-        <v>146</v>
+        <v>175</v>
       </c>
       <c r="C53" t="s">
-        <v>147</v>
+        <v>176</v>
       </c>
       <c r="D53" t="s">
-        <v>148</v>
+        <v>177</v>
       </c>
       <c r="E53" t="s">
         <v>104</v>
@@ -2943,13 +2961,13 @@
         <v>56</v>
       </c>
       <c r="B54" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C54" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D54" t="s">
-        <v>378</v>
+        <v>148</v>
       </c>
       <c r="E54" t="s">
         <v>104</v>
@@ -2960,13 +2978,13 @@
         <v>56</v>
       </c>
       <c r="B55" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="C55" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="D55" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="E55" t="s">
         <v>104</v>
@@ -2977,13 +2995,13 @@
         <v>56</v>
       </c>
       <c r="B56" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C56" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D56" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E56" t="s">
         <v>104</v>
@@ -2994,13 +3012,13 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C57" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D57" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E57" t="s">
         <v>104</v>
@@ -3011,13 +3029,13 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C58" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="D58" t="s">
-        <v>162</v>
+        <v>377</v>
       </c>
       <c r="E58" t="s">
         <v>104</v>
@@ -3028,13 +3046,13 @@
         <v>56</v>
       </c>
       <c r="B59" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
       <c r="C59" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="D59" t="s">
-        <v>380</v>
+        <v>162</v>
       </c>
       <c r="E59" t="s">
         <v>104</v>
@@ -3045,13 +3063,13 @@
         <v>56</v>
       </c>
       <c r="B60" t="s">
-        <v>189</v>
+        <v>149</v>
       </c>
       <c r="C60" t="s">
-        <v>190</v>
+        <v>150</v>
       </c>
       <c r="D60" t="s">
-        <v>354</v>
+        <v>380</v>
       </c>
       <c r="E60" t="s">
         <v>104</v>
@@ -3062,13 +3080,13 @@
         <v>56</v>
       </c>
       <c r="B61" t="s">
-        <v>166</v>
+        <v>189</v>
       </c>
       <c r="C61" t="s">
-        <v>167</v>
+        <v>190</v>
       </c>
       <c r="D61" t="s">
-        <v>168</v>
+        <v>354</v>
       </c>
       <c r="E61" t="s">
         <v>104</v>
@@ -3079,13 +3097,13 @@
         <v>56</v>
       </c>
       <c r="B62" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C62" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="D62" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="E62" t="s">
         <v>104</v>
@@ -3096,13 +3114,13 @@
         <v>56</v>
       </c>
       <c r="B63" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C63" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="D63" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="E63" t="s">
         <v>104</v>
@@ -3113,13 +3131,13 @@
         <v>56</v>
       </c>
       <c r="B64" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="C64" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="D64" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="E64" t="s">
         <v>104</v>
@@ -3130,13 +3148,13 @@
         <v>56</v>
       </c>
       <c r="B65" t="s">
-        <v>439</v>
+        <v>169</v>
       </c>
       <c r="C65" t="s">
-        <v>438</v>
+        <v>170</v>
       </c>
       <c r="D65" t="s">
-        <v>422</v>
+        <v>171</v>
       </c>
       <c r="E65" t="s">
         <v>104</v>
@@ -3147,13 +3165,13 @@
         <v>56</v>
       </c>
       <c r="B66" t="s">
-        <v>451</v>
+        <v>439</v>
       </c>
       <c r="C66" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="D66" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E66" t="s">
         <v>104</v>
@@ -3164,13 +3182,13 @@
         <v>56</v>
       </c>
       <c r="B67" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="C67" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
       <c r="D67" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E67" t="s">
         <v>104</v>
@@ -3181,13 +3199,13 @@
         <v>56</v>
       </c>
       <c r="B68" t="s">
-        <v>444</v>
+        <v>450</v>
       </c>
       <c r="C68" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="D68" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E68" t="s">
         <v>104</v>
@@ -3198,16 +3216,16 @@
         <v>56</v>
       </c>
       <c r="B69" t="s">
-        <v>206</v>
+        <v>444</v>
       </c>
       <c r="C69" t="s">
-        <v>207</v>
+        <v>445</v>
       </c>
       <c r="D69" t="s">
-        <v>357</v>
+        <v>425</v>
       </c>
       <c r="E69" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -3215,13 +3233,13 @@
         <v>56</v>
       </c>
       <c r="B70" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="C70" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="D70" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="E70" t="s">
         <v>106</v>
@@ -3232,13 +3250,13 @@
         <v>56</v>
       </c>
       <c r="B71" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="C71" t="s">
-        <v>458</v>
+        <v>214</v>
       </c>
       <c r="D71" t="s">
-        <v>385</v>
+        <v>359</v>
       </c>
       <c r="E71" t="s">
         <v>106</v>
@@ -3249,13 +3267,13 @@
         <v>56</v>
       </c>
       <c r="B72" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C72" t="s">
-        <v>467</v>
+        <v>458</v>
       </c>
       <c r="D72" t="s">
-        <v>364</v>
+        <v>385</v>
       </c>
       <c r="E72" t="s">
         <v>106</v>
@@ -3266,13 +3284,13 @@
         <v>56</v>
       </c>
       <c r="B73" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="C73" t="s">
-        <v>454</v>
+        <v>467</v>
       </c>
       <c r="D73" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="E73" t="s">
         <v>106</v>
@@ -3283,13 +3301,13 @@
         <v>56</v>
       </c>
       <c r="B74" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="C74" t="s">
-        <v>466</v>
+        <v>454</v>
       </c>
       <c r="D74" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="E74" t="s">
         <v>106</v>
@@ -3300,13 +3318,13 @@
         <v>56</v>
       </c>
       <c r="B75" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="C75" t="s">
-        <v>223</v>
+        <v>466</v>
       </c>
       <c r="D75" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="E75" t="s">
         <v>106</v>
@@ -3317,13 +3335,13 @@
         <v>56</v>
       </c>
       <c r="B76" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C76" t="s">
-        <v>457</v>
+        <v>223</v>
       </c>
       <c r="D76" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E76" t="s">
         <v>106</v>
@@ -3334,13 +3352,13 @@
         <v>56</v>
       </c>
       <c r="B77" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C77" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
       <c r="D77" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="E77" t="s">
         <v>106</v>
@@ -3351,13 +3369,13 @@
         <v>56</v>
       </c>
       <c r="B78" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C78" t="s">
-        <v>462</v>
+        <v>453</v>
       </c>
       <c r="D78" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E78" t="s">
         <v>106</v>
@@ -3368,13 +3386,13 @@
         <v>56</v>
       </c>
       <c r="B79" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="C79" t="s">
-        <v>455</v>
+        <v>462</v>
       </c>
       <c r="D79" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="E79" t="s">
         <v>106</v>
@@ -3385,13 +3403,13 @@
         <v>56</v>
       </c>
       <c r="B80" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C80" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="D80" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E80" t="s">
         <v>106</v>
@@ -3402,13 +3420,13 @@
         <v>56</v>
       </c>
       <c r="B81" t="s">
-        <v>205</v>
+        <v>226</v>
       </c>
       <c r="C81" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D81" t="s">
-        <v>356</v>
+        <v>368</v>
       </c>
       <c r="E81" t="s">
         <v>106</v>
@@ -3419,13 +3437,13 @@
         <v>56</v>
       </c>
       <c r="B82" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="C82" t="s">
-        <v>204</v>
+        <v>460</v>
       </c>
       <c r="D82" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="E82" t="s">
         <v>106</v>
@@ -3436,13 +3454,13 @@
         <v>56</v>
       </c>
       <c r="B83" t="s">
-        <v>229</v>
+        <v>203</v>
       </c>
       <c r="C83" t="s">
-        <v>456</v>
+        <v>204</v>
       </c>
       <c r="D83" t="s">
-        <v>371</v>
+        <v>355</v>
       </c>
       <c r="E83" t="s">
         <v>106</v>
@@ -3453,13 +3471,13 @@
         <v>56</v>
       </c>
       <c r="B84" t="s">
-        <v>219</v>
+        <v>229</v>
       </c>
       <c r="C84" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
       <c r="D84" t="s">
-        <v>363</v>
+        <v>371</v>
       </c>
       <c r="E84" t="s">
         <v>106</v>
@@ -3470,13 +3488,13 @@
         <v>56</v>
       </c>
       <c r="B85" t="s">
-        <v>397</v>
+        <v>219</v>
       </c>
       <c r="C85" t="s">
-        <v>464</v>
+        <v>452</v>
       </c>
       <c r="D85" t="s">
-        <v>398</v>
+        <v>363</v>
       </c>
       <c r="E85" t="s">
         <v>106</v>
@@ -3487,13 +3505,13 @@
         <v>56</v>
       </c>
       <c r="B86" t="s">
-        <v>217</v>
+        <v>397</v>
       </c>
       <c r="C86" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D86" t="s">
-        <v>387</v>
+        <v>398</v>
       </c>
       <c r="E86" t="s">
         <v>106</v>
@@ -3504,13 +3522,13 @@
         <v>56</v>
       </c>
       <c r="B87" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C87" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="D87" t="s">
-        <v>362</v>
+        <v>387</v>
       </c>
       <c r="E87" t="s">
         <v>106</v>
@@ -3521,13 +3539,13 @@
         <v>56</v>
       </c>
       <c r="B88" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C88" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D88" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="E88" t="s">
         <v>106</v>
@@ -3538,13 +3556,13 @@
         <v>56</v>
       </c>
       <c r="B89" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="C89" t="s">
-        <v>461</v>
+        <v>471</v>
       </c>
       <c r="D89" t="s">
-        <v>382</v>
+        <v>361</v>
       </c>
       <c r="E89" t="s">
         <v>106</v>
@@ -3555,13 +3573,13 @@
         <v>56</v>
       </c>
       <c r="B90" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C90" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D90" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E90" t="s">
         <v>106</v>
@@ -3572,13 +3590,13 @@
         <v>56</v>
       </c>
       <c r="B91" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C91" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="D91" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="E91" t="s">
         <v>106</v>
@@ -3589,13 +3607,13 @@
         <v>56</v>
       </c>
       <c r="B92" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C92" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D92" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="E92" t="s">
         <v>106</v>
@@ -3606,16 +3624,16 @@
         <v>56</v>
       </c>
       <c r="B93" t="s">
-        <v>261</v>
+        <v>211</v>
       </c>
       <c r="C93" t="s">
-        <v>262</v>
+        <v>469</v>
       </c>
       <c r="D93" t="s">
-        <v>435</v>
+        <v>384</v>
       </c>
       <c r="E93" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -3623,16 +3641,16 @@
         <v>56</v>
       </c>
       <c r="B94" t="s">
-        <v>263</v>
+        <v>477</v>
       </c>
       <c r="C94" t="s">
-        <v>264</v>
+        <v>479</v>
       </c>
       <c r="D94" t="s">
-        <v>436</v>
+        <v>481</v>
       </c>
       <c r="E94" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -3640,16 +3658,16 @@
         <v>56</v>
       </c>
       <c r="B95" t="s">
-        <v>301</v>
+        <v>478</v>
       </c>
       <c r="C95" t="s">
-        <v>302</v>
+        <v>480</v>
       </c>
       <c r="D95" t="s">
-        <v>386</v>
+        <v>482</v>
       </c>
       <c r="E95" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -3657,13 +3675,13 @@
         <v>56</v>
       </c>
       <c r="B96" t="s">
-        <v>319</v>
+        <v>261</v>
       </c>
       <c r="C96" t="s">
-        <v>320</v>
+        <v>262</v>
       </c>
       <c r="D96" t="s">
-        <v>321</v>
+        <v>435</v>
       </c>
       <c r="E96" t="s">
         <v>108</v>
@@ -3674,13 +3692,13 @@
         <v>56</v>
       </c>
       <c r="B97" t="s">
-        <v>400</v>
+        <v>263</v>
       </c>
       <c r="C97" t="s">
-        <v>236</v>
+        <v>264</v>
       </c>
       <c r="D97" t="s">
-        <v>237</v>
+        <v>436</v>
       </c>
       <c r="E97" t="s">
         <v>108</v>
@@ -3691,13 +3709,13 @@
         <v>56</v>
       </c>
       <c r="B98" t="s">
-        <v>430</v>
+        <v>301</v>
       </c>
       <c r="C98" t="s">
-        <v>409</v>
+        <v>302</v>
       </c>
       <c r="D98" t="s">
-        <v>410</v>
+        <v>386</v>
       </c>
       <c r="E98" t="s">
         <v>108</v>
@@ -3708,13 +3726,13 @@
         <v>56</v>
       </c>
       <c r="B99" t="s">
-        <v>298</v>
+        <v>319</v>
       </c>
       <c r="C99" t="s">
-        <v>299</v>
+        <v>320</v>
       </c>
       <c r="D99" t="s">
-        <v>300</v>
+        <v>321</v>
       </c>
       <c r="E99" t="s">
         <v>108</v>
@@ -3725,13 +3743,13 @@
         <v>56</v>
       </c>
       <c r="B100" t="s">
-        <v>248</v>
+        <v>400</v>
       </c>
       <c r="C100" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="D100" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="E100" t="s">
         <v>108</v>
@@ -3742,13 +3760,13 @@
         <v>56</v>
       </c>
       <c r="B101" t="s">
-        <v>230</v>
+        <v>430</v>
       </c>
       <c r="C101" t="s">
-        <v>231</v>
+        <v>409</v>
       </c>
       <c r="D101" t="s">
-        <v>232</v>
+        <v>410</v>
       </c>
       <c r="E101" t="s">
         <v>108</v>
@@ -3759,13 +3777,13 @@
         <v>56</v>
       </c>
       <c r="B102" t="s">
-        <v>428</v>
+        <v>298</v>
       </c>
       <c r="C102" t="s">
-        <v>405</v>
+        <v>299</v>
       </c>
       <c r="D102" t="s">
-        <v>406</v>
+        <v>300</v>
       </c>
       <c r="E102" t="s">
         <v>108</v>
@@ -3776,13 +3794,13 @@
         <v>56</v>
       </c>
       <c r="B103" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="C103" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="D103" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="E103" t="s">
         <v>108</v>
@@ -3793,13 +3811,13 @@
         <v>56</v>
       </c>
       <c r="B104" t="s">
-        <v>265</v>
+        <v>230</v>
       </c>
       <c r="C104" t="s">
-        <v>266</v>
+        <v>231</v>
       </c>
       <c r="D104" t="s">
-        <v>420</v>
+        <v>232</v>
       </c>
       <c r="E104" t="s">
         <v>108</v>
@@ -3810,13 +3828,13 @@
         <v>56</v>
       </c>
       <c r="B105" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
       <c r="C105" t="s">
-        <v>415</v>
+        <v>405</v>
       </c>
       <c r="D105" t="s">
-        <v>437</v>
+        <v>406</v>
       </c>
       <c r="E105" t="s">
         <v>108</v>
@@ -3827,13 +3845,13 @@
         <v>56</v>
       </c>
       <c r="B106" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="C106" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="D106" t="s">
-        <v>390</v>
+        <v>260</v>
       </c>
       <c r="E106" t="s">
         <v>108</v>
@@ -3844,13 +3862,13 @@
         <v>56</v>
       </c>
       <c r="B107" t="s">
-        <v>251</v>
+        <v>265</v>
       </c>
       <c r="C107" t="s">
-        <v>252</v>
+        <v>266</v>
       </c>
       <c r="D107" t="s">
-        <v>389</v>
+        <v>420</v>
       </c>
       <c r="E107" t="s">
         <v>108</v>
@@ -3861,13 +3879,13 @@
         <v>56</v>
       </c>
       <c r="B108" t="s">
-        <v>309</v>
+        <v>434</v>
       </c>
       <c r="C108" t="s">
-        <v>310</v>
+        <v>415</v>
       </c>
       <c r="D108" t="s">
-        <v>311</v>
+        <v>437</v>
       </c>
       <c r="E108" t="s">
         <v>108</v>
@@ -3878,13 +3896,13 @@
         <v>56</v>
       </c>
       <c r="B109" t="s">
-        <v>245</v>
+        <v>256</v>
       </c>
       <c r="C109" t="s">
-        <v>246</v>
+        <v>257</v>
       </c>
       <c r="D109" t="s">
-        <v>247</v>
+        <v>390</v>
       </c>
       <c r="E109" t="s">
         <v>108</v>
@@ -3895,13 +3913,13 @@
         <v>56</v>
       </c>
       <c r="B110" t="s">
-        <v>292</v>
+        <v>251</v>
       </c>
       <c r="C110" t="s">
-        <v>293</v>
+        <v>252</v>
       </c>
       <c r="D110" t="s">
-        <v>294</v>
+        <v>389</v>
       </c>
       <c r="E110" t="s">
         <v>108</v>
@@ -3912,13 +3930,13 @@
         <v>56</v>
       </c>
       <c r="B111" t="s">
-        <v>233</v>
+        <v>309</v>
       </c>
       <c r="C111" t="s">
-        <v>234</v>
+        <v>310</v>
       </c>
       <c r="D111" t="s">
-        <v>235</v>
+        <v>311</v>
       </c>
       <c r="E111" t="s">
         <v>108</v>
@@ -3929,13 +3947,13 @@
         <v>56</v>
       </c>
       <c r="B112" t="s">
-        <v>429</v>
+        <v>245</v>
       </c>
       <c r="C112" t="s">
-        <v>407</v>
+        <v>246</v>
       </c>
       <c r="D112" t="s">
-        <v>408</v>
+        <v>247</v>
       </c>
       <c r="E112" t="s">
         <v>108</v>
@@ -3946,13 +3964,13 @@
         <v>56</v>
       </c>
       <c r="B113" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C113" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D113" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="E113" t="s">
         <v>108</v>
@@ -3963,13 +3981,13 @@
         <v>56</v>
       </c>
       <c r="B114" t="s">
-        <v>322</v>
+        <v>233</v>
       </c>
       <c r="C114" t="s">
-        <v>323</v>
+        <v>234</v>
       </c>
       <c r="D114" t="s">
-        <v>324</v>
+        <v>235</v>
       </c>
       <c r="E114" t="s">
         <v>108</v>
@@ -3980,13 +3998,13 @@
         <v>56</v>
       </c>
       <c r="B115" t="s">
-        <v>241</v>
+        <v>429</v>
       </c>
       <c r="C115" t="s">
-        <v>242</v>
+        <v>407</v>
       </c>
       <c r="D115" t="s">
-        <v>418</v>
+        <v>408</v>
       </c>
       <c r="E115" t="s">
         <v>108</v>
@@ -3997,13 +4015,13 @@
         <v>56</v>
       </c>
       <c r="B116" t="s">
-        <v>432</v>
+        <v>295</v>
       </c>
       <c r="C116" t="s">
-        <v>413</v>
+        <v>296</v>
       </c>
       <c r="D116" t="s">
-        <v>416</v>
+        <v>297</v>
       </c>
       <c r="E116" t="s">
         <v>108</v>
@@ -4014,13 +4032,13 @@
         <v>56</v>
       </c>
       <c r="B117" t="s">
-        <v>280</v>
+        <v>322</v>
       </c>
       <c r="C117" t="s">
-        <v>281</v>
+        <v>323</v>
       </c>
       <c r="D117" t="s">
-        <v>282</v>
+        <v>324</v>
       </c>
       <c r="E117" t="s">
         <v>108</v>
@@ -4031,13 +4049,13 @@
         <v>56</v>
       </c>
       <c r="B118" t="s">
-        <v>286</v>
+        <v>241</v>
       </c>
       <c r="C118" t="s">
-        <v>287</v>
+        <v>242</v>
       </c>
       <c r="D118" t="s">
-        <v>288</v>
+        <v>418</v>
       </c>
       <c r="E118" t="s">
         <v>108</v>
@@ -4048,13 +4066,13 @@
         <v>56</v>
       </c>
       <c r="B119" t="s">
-        <v>283</v>
+        <v>432</v>
       </c>
       <c r="C119" t="s">
-        <v>284</v>
+        <v>413</v>
       </c>
       <c r="D119" t="s">
-        <v>285</v>
+        <v>416</v>
       </c>
       <c r="E119" t="s">
         <v>108</v>
@@ -4065,13 +4083,13 @@
         <v>56</v>
       </c>
       <c r="B120" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="C120" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="D120" t="s">
-        <v>372</v>
+        <v>282</v>
       </c>
       <c r="E120" t="s">
         <v>108</v>
@@ -4082,13 +4100,13 @@
         <v>56</v>
       </c>
       <c r="B121" t="s">
-        <v>267</v>
+        <v>286</v>
       </c>
       <c r="C121" t="s">
-        <v>268</v>
+        <v>287</v>
       </c>
       <c r="D121" t="s">
-        <v>421</v>
+        <v>288</v>
       </c>
       <c r="E121" t="s">
         <v>108</v>
@@ -4099,13 +4117,13 @@
         <v>56</v>
       </c>
       <c r="B122" t="s">
-        <v>271</v>
+        <v>283</v>
       </c>
       <c r="C122" t="s">
-        <v>272</v>
+        <v>284</v>
       </c>
       <c r="D122" t="s">
-        <v>427</v>
+        <v>285</v>
       </c>
       <c r="E122" t="s">
         <v>108</v>
@@ -4116,13 +4134,13 @@
         <v>56</v>
       </c>
       <c r="B123" t="s">
-        <v>269</v>
+        <v>276</v>
       </c>
       <c r="C123" t="s">
-        <v>270</v>
+        <v>277</v>
       </c>
       <c r="D123" t="s">
-        <v>426</v>
+        <v>372</v>
       </c>
       <c r="E123" t="s">
         <v>108</v>
@@ -4133,13 +4151,13 @@
         <v>56</v>
       </c>
       <c r="B124" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="C124" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
       <c r="D124" t="s">
-        <v>291</v>
+        <v>373</v>
       </c>
       <c r="E124" t="s">
         <v>108</v>
@@ -4150,13 +4168,13 @@
         <v>56</v>
       </c>
       <c r="B125" t="s">
-        <v>238</v>
+        <v>267</v>
       </c>
       <c r="C125" t="s">
-        <v>239</v>
+        <v>268</v>
       </c>
       <c r="D125" t="s">
-        <v>240</v>
+        <v>421</v>
       </c>
       <c r="E125" t="s">
         <v>108</v>
@@ -4167,13 +4185,13 @@
         <v>56</v>
       </c>
       <c r="B126" t="s">
-        <v>431</v>
+        <v>271</v>
       </c>
       <c r="C126" t="s">
-        <v>411</v>
+        <v>272</v>
       </c>
       <c r="D126" t="s">
-        <v>412</v>
+        <v>427</v>
       </c>
       <c r="E126" t="s">
         <v>108</v>
@@ -4184,13 +4202,13 @@
         <v>56</v>
       </c>
       <c r="B127" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="C127" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="D127" t="s">
-        <v>373</v>
+        <v>426</v>
       </c>
       <c r="E127" t="s">
         <v>108</v>
@@ -4201,13 +4219,13 @@
         <v>56</v>
       </c>
       <c r="B128" t="s">
-        <v>273</v>
+        <v>289</v>
       </c>
       <c r="C128" t="s">
-        <v>274</v>
+        <v>290</v>
       </c>
       <c r="D128" t="s">
-        <v>275</v>
+        <v>291</v>
       </c>
       <c r="E128" t="s">
         <v>108</v>
@@ -4218,13 +4236,13 @@
         <v>56</v>
       </c>
       <c r="B129" t="s">
-        <v>303</v>
+        <v>238</v>
       </c>
       <c r="C129" t="s">
-        <v>304</v>
+        <v>239</v>
       </c>
       <c r="D129" t="s">
-        <v>305</v>
+        <v>240</v>
       </c>
       <c r="E129" t="s">
         <v>108</v>
@@ -4235,13 +4253,13 @@
         <v>56</v>
       </c>
       <c r="B130" t="s">
-        <v>318</v>
+        <v>431</v>
       </c>
       <c r="C130" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="D130" t="s">
-        <v>403</v>
+        <v>412</v>
       </c>
       <c r="E130" t="s">
         <v>108</v>
@@ -4252,13 +4270,13 @@
         <v>56</v>
       </c>
       <c r="B131" t="s">
-        <v>315</v>
+        <v>273</v>
       </c>
       <c r="C131" t="s">
-        <v>316</v>
+        <v>274</v>
       </c>
       <c r="D131" t="s">
-        <v>317</v>
+        <v>275</v>
       </c>
       <c r="E131" t="s">
         <v>108</v>
@@ -4269,13 +4287,13 @@
         <v>56</v>
       </c>
       <c r="B132" t="s">
-        <v>253</v>
+        <v>303</v>
       </c>
       <c r="C132" t="s">
-        <v>254</v>
+        <v>304</v>
       </c>
       <c r="D132" t="s">
-        <v>255</v>
+        <v>305</v>
       </c>
       <c r="E132" t="s">
         <v>108</v>
@@ -4286,13 +4304,13 @@
         <v>56</v>
       </c>
       <c r="B133" t="s">
-        <v>243</v>
+        <v>318</v>
       </c>
       <c r="C133" t="s">
-        <v>244</v>
+        <v>404</v>
       </c>
       <c r="D133" t="s">
-        <v>419</v>
+        <v>403</v>
       </c>
       <c r="E133" t="s">
         <v>108</v>
@@ -4303,13 +4321,13 @@
         <v>56</v>
       </c>
       <c r="B134" t="s">
-        <v>433</v>
+        <v>315</v>
       </c>
       <c r="C134" t="s">
-        <v>414</v>
+        <v>316</v>
       </c>
       <c r="D134" t="s">
-        <v>417</v>
+        <v>317</v>
       </c>
       <c r="E134" t="s">
         <v>108</v>
@@ -4320,13 +4338,13 @@
         <v>56</v>
       </c>
       <c r="B135" t="s">
-        <v>312</v>
+        <v>253</v>
       </c>
       <c r="C135" t="s">
-        <v>313</v>
+        <v>254</v>
       </c>
       <c r="D135" t="s">
-        <v>314</v>
+        <v>255</v>
       </c>
       <c r="E135" t="s">
         <v>108</v>
@@ -4337,13 +4355,13 @@
         <v>56</v>
       </c>
       <c r="B136" t="s">
-        <v>306</v>
+        <v>243</v>
       </c>
       <c r="C136" t="s">
-        <v>307</v>
+        <v>244</v>
       </c>
       <c r="D136" t="s">
-        <v>308</v>
+        <v>419</v>
       </c>
       <c r="E136" t="s">
         <v>108</v>
@@ -4354,21 +4372,72 @@
         <v>56</v>
       </c>
       <c r="B137" t="s">
-        <v>401</v>
+        <v>433</v>
       </c>
       <c r="C137" t="s">
-        <v>402</v>
+        <v>414</v>
       </c>
       <c r="D137" t="s">
-        <v>388</v>
+        <v>417</v>
       </c>
       <c r="E137" t="s">
         <v>108</v>
       </c>
     </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>56</v>
+      </c>
+      <c r="B138" t="s">
+        <v>312</v>
+      </c>
+      <c r="C138" t="s">
+        <v>313</v>
+      </c>
+      <c r="D138" t="s">
+        <v>314</v>
+      </c>
+      <c r="E138" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>56</v>
+      </c>
+      <c r="B139" t="s">
+        <v>306</v>
+      </c>
+      <c r="C139" t="s">
+        <v>307</v>
+      </c>
+      <c r="D139" t="s">
+        <v>308</v>
+      </c>
+      <c r="E139" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>56</v>
+      </c>
+      <c r="B140" t="s">
+        <v>401</v>
+      </c>
+      <c r="C140" t="s">
+        <v>402</v>
+      </c>
+      <c r="D140" t="s">
+        <v>388</v>
+      </c>
+      <c r="E140" t="s">
+        <v>108</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A93:E137">
-    <sortCondition ref="C93:C137"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A96:E140">
+    <sortCondition ref="C96:C140"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Add key for icon colors
</commit_message>
<xml_diff>
--- a/form.xlsx
+++ b/form.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\aerialsurvey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54016476-EFBE-47B3-B144-524BCA9ED9CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9894638-CF30-4B92-968A-F48D885F155A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11205" yWindow="1545" windowWidth="35190" windowHeight="12690" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11205" yWindow="0" windowWidth="35190" windowHeight="20985" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="481">
   <si>
     <t>type</t>
   </si>
@@ -262,12 +262,6 @@
   </si>
   <si>
     <t>Falk</t>
-  </si>
-  <si>
-    <t>justin</t>
-  </si>
-  <si>
-    <t>Justin</t>
   </si>
   <si>
     <t>richard</t>
@@ -1818,7 +1812,7 @@
   <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1856,7 +1850,7 @@
         <v>9</v>
       </c>
       <c r="F1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
@@ -1865,7 +1859,7 @@
         <v>5</v>
       </c>
       <c r="I1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="J1" t="s">
         <v>6</v>
@@ -1897,10 +1891,10 @@
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D2" t="s">
         <v>15</v>
@@ -1937,7 +1931,7 @@
         <v>22</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="J4" t="s">
         <v>23</v>
@@ -1974,7 +1968,7 @@
         <v>29</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="J6" t="s">
         <v>23</v>
@@ -2010,19 +2004,25 @@
       <c r="D8" t="s">
         <v>35</v>
       </c>
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
       <c r="B9" t="s">
+        <v>348</v>
+      </c>
+      <c r="C9" t="s">
+        <v>349</v>
+      </c>
+      <c r="E9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" t="s">
         <v>350</v>
-      </c>
-      <c r="C9" t="s">
-        <v>351</v>
-      </c>
-      <c r="F9" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -2044,13 +2044,13 @@
         <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C11" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="F11" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -2072,13 +2072,13 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
+        <v>338</v>
+      </c>
+      <c r="C13" t="s">
         <v>340</v>
       </c>
-      <c r="C13" t="s">
-        <v>342</v>
-      </c>
       <c r="F13" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -2100,13 +2100,13 @@
         <v>20</v>
       </c>
       <c r="B15" t="s">
+        <v>339</v>
+      </c>
+      <c r="C15" t="s">
         <v>341</v>
       </c>
-      <c r="C15" t="s">
-        <v>343</v>
-      </c>
       <c r="F15" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
@@ -2122,6 +2122,9 @@
       <c r="D16" t="s">
         <v>35</v>
       </c>
+      <c r="E16" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -2133,6 +2136,9 @@
       <c r="C17" t="s">
         <v>46</v>
       </c>
+      <c r="E17" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -2159,7 +2165,7 @@
         <v>35</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="J19" t="s">
         <v>23</v>
@@ -2260,10 +2266,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E140"/>
+  <dimension ref="A1:E139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A117" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A125" sqref="A125"/>
+    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2296,10 +2302,10 @@
         <v>73</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>474</v>
       </c>
       <c r="C2" t="s">
-        <v>75</v>
+        <v>473</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2307,10 +2313,10 @@
         <v>73</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2318,10 +2324,10 @@
         <v>73</v>
       </c>
       <c r="B4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2329,10 +2335,10 @@
         <v>73</v>
       </c>
       <c r="B5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2340,10 +2346,10 @@
         <v>73</v>
       </c>
       <c r="B6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2351,21 +2357,21 @@
         <v>73</v>
       </c>
       <c r="B7" t="s">
-        <v>476</v>
+        <v>334</v>
       </c>
       <c r="C7" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>73</v>
-      </c>
-      <c r="B8" t="s">
-        <v>336</v>
-      </c>
-      <c r="C8" t="s">
-        <v>337</v>
+        <v>335</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2401,14 +2407,14 @@
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" t="s">
         <v>90</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2417,21 +2423,21 @@
         <v>60</v>
       </c>
       <c r="B15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" t="s">
         <v>92</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C17" t="s">
         <v>93</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>60</v>
-      </c>
-      <c r="B16" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2445,14 +2451,14 @@
         <v>95</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>66</v>
-      </c>
-      <c r="B19" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" t="s">
         <v>96</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>97</v>
       </c>
     </row>
@@ -2478,15 +2484,18 @@
         <v>101</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>69</v>
-      </c>
-      <c r="B23" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" t="s">
         <v>102</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>103</v>
+      </c>
+      <c r="D24" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -2511,24 +2520,27 @@
         <v>106</v>
       </c>
       <c r="C26" t="s">
-        <v>107</v>
+        <v>397</v>
       </c>
       <c r="D26" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>50</v>
-      </c>
-      <c r="B27" t="s">
-        <v>108</v>
-      </c>
-      <c r="C27" t="s">
-        <v>399</v>
-      </c>
-      <c r="D27" t="s">
-        <v>473</v>
+        <v>471</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" t="s">
+        <v>439</v>
+      </c>
+      <c r="C28" t="s">
+        <v>440</v>
+      </c>
+      <c r="D28" t="s">
+        <v>389</v>
+      </c>
+      <c r="E28" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -2536,16 +2548,16 @@
         <v>56</v>
       </c>
       <c r="B29" t="s">
-        <v>441</v>
+        <v>186</v>
       </c>
       <c r="C29" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="D29" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E29" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -2553,16 +2565,16 @@
         <v>56</v>
       </c>
       <c r="B30" t="s">
-        <v>188</v>
+        <v>113</v>
       </c>
       <c r="C30" t="s">
-        <v>446</v>
+        <v>114</v>
       </c>
       <c r="D30" t="s">
-        <v>392</v>
+        <v>115</v>
       </c>
       <c r="E30" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -2570,16 +2582,16 @@
         <v>56</v>
       </c>
       <c r="B31" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C31" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="D31" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="E31" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -2587,16 +2599,16 @@
         <v>56</v>
       </c>
       <c r="B32" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C32" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D32" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E32" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -2604,16 +2616,16 @@
         <v>56</v>
       </c>
       <c r="B33" t="s">
-        <v>112</v>
+        <v>176</v>
       </c>
       <c r="C33" t="s">
-        <v>113</v>
+        <v>177</v>
       </c>
       <c r="D33" t="s">
-        <v>114</v>
+        <v>178</v>
       </c>
       <c r="E33" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -2621,16 +2633,16 @@
         <v>56</v>
       </c>
       <c r="B34" t="s">
-        <v>178</v>
+        <v>116</v>
       </c>
       <c r="C34" t="s">
-        <v>179</v>
+        <v>117</v>
       </c>
       <c r="D34" t="s">
-        <v>180</v>
+        <v>118</v>
       </c>
       <c r="E34" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -2638,16 +2650,16 @@
         <v>56</v>
       </c>
       <c r="B35" t="s">
-        <v>118</v>
+        <v>189</v>
       </c>
       <c r="C35" t="s">
-        <v>119</v>
+        <v>190</v>
       </c>
       <c r="D35" t="s">
-        <v>120</v>
+        <v>191</v>
       </c>
       <c r="E35" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -2655,16 +2667,16 @@
         <v>56</v>
       </c>
       <c r="B36" t="s">
-        <v>191</v>
+        <v>119</v>
       </c>
       <c r="C36" t="s">
-        <v>192</v>
+        <v>120</v>
       </c>
       <c r="D36" t="s">
-        <v>193</v>
+        <v>351</v>
       </c>
       <c r="E36" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -2678,10 +2690,10 @@
         <v>122</v>
       </c>
       <c r="D37" t="s">
-        <v>353</v>
+        <v>123</v>
       </c>
       <c r="E37" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -2689,16 +2701,16 @@
         <v>56</v>
       </c>
       <c r="B38" t="s">
-        <v>123</v>
+        <v>198</v>
       </c>
       <c r="C38" t="s">
-        <v>124</v>
+        <v>199</v>
       </c>
       <c r="D38" t="s">
-        <v>125</v>
+        <v>200</v>
       </c>
       <c r="E38" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -2706,16 +2718,16 @@
         <v>56</v>
       </c>
       <c r="B39" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C39" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="D39" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="E39" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -2723,16 +2735,16 @@
         <v>56</v>
       </c>
       <c r="B40" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C40" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="D40" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="E40" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -2740,16 +2752,16 @@
         <v>56</v>
       </c>
       <c r="B41" t="s">
-        <v>194</v>
+        <v>127</v>
       </c>
       <c r="C41" t="s">
-        <v>195</v>
+        <v>128</v>
       </c>
       <c r="D41" t="s">
-        <v>196</v>
+        <v>129</v>
       </c>
       <c r="E41" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -2757,16 +2769,16 @@
         <v>56</v>
       </c>
       <c r="B42" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C42" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D42" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E42" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -2774,16 +2786,16 @@
         <v>56</v>
       </c>
       <c r="B43" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="C43" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="D43" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="E43" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -2791,16 +2803,16 @@
         <v>56</v>
       </c>
       <c r="B44" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C44" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D44" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E44" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -2808,16 +2820,16 @@
         <v>56</v>
       </c>
       <c r="B45" t="s">
-        <v>135</v>
+        <v>184</v>
       </c>
       <c r="C45" t="s">
-        <v>136</v>
+        <v>445</v>
       </c>
       <c r="D45" t="s">
-        <v>137</v>
+        <v>185</v>
       </c>
       <c r="E45" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -2825,16 +2837,16 @@
         <v>56</v>
       </c>
       <c r="B46" t="s">
-        <v>186</v>
+        <v>155</v>
       </c>
       <c r="C46" t="s">
-        <v>447</v>
+        <v>156</v>
       </c>
       <c r="D46" t="s">
-        <v>187</v>
+        <v>157</v>
       </c>
       <c r="E46" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -2842,16 +2854,16 @@
         <v>56</v>
       </c>
       <c r="B47" t="s">
-        <v>157</v>
+        <v>182</v>
       </c>
       <c r="C47" t="s">
-        <v>158</v>
+        <v>183</v>
       </c>
       <c r="D47" t="s">
-        <v>159</v>
+        <v>377</v>
       </c>
       <c r="E47" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -2859,16 +2871,16 @@
         <v>56</v>
       </c>
       <c r="B48" t="s">
-        <v>184</v>
+        <v>136</v>
       </c>
       <c r="C48" t="s">
-        <v>185</v>
+        <v>137</v>
       </c>
       <c r="D48" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
       <c r="E48" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -2876,16 +2888,16 @@
         <v>56</v>
       </c>
       <c r="B49" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C49" t="s">
-        <v>139</v>
+        <v>447</v>
       </c>
       <c r="D49" t="s">
-        <v>374</v>
+        <v>141</v>
       </c>
       <c r="E49" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -2893,16 +2905,16 @@
         <v>56</v>
       </c>
       <c r="B50" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C50" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="D50" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E50" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -2910,16 +2922,16 @@
         <v>56</v>
       </c>
       <c r="B51" t="s">
-        <v>140</v>
+        <v>179</v>
       </c>
       <c r="C51" t="s">
-        <v>448</v>
+        <v>180</v>
       </c>
       <c r="D51" t="s">
-        <v>141</v>
+        <v>181</v>
       </c>
       <c r="E51" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -2927,16 +2939,16 @@
         <v>56</v>
       </c>
       <c r="B52" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="C52" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="D52" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="E52" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -2944,16 +2956,16 @@
         <v>56</v>
       </c>
       <c r="B53" t="s">
-        <v>175</v>
+        <v>144</v>
       </c>
       <c r="C53" t="s">
-        <v>176</v>
+        <v>145</v>
       </c>
       <c r="D53" t="s">
-        <v>177</v>
+        <v>146</v>
       </c>
       <c r="E53" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -2961,16 +2973,16 @@
         <v>56</v>
       </c>
       <c r="B54" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C54" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D54" t="s">
-        <v>148</v>
+        <v>376</v>
       </c>
       <c r="E54" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -2978,16 +2990,16 @@
         <v>56</v>
       </c>
       <c r="B55" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="C55" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="D55" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="E55" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -3001,10 +3013,10 @@
         <v>152</v>
       </c>
       <c r="D56" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E56" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -3018,10 +3030,10 @@
         <v>154</v>
       </c>
       <c r="D57" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E57" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -3029,16 +3041,16 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C58" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="D58" t="s">
-        <v>377</v>
+        <v>160</v>
       </c>
       <c r="E58" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -3046,16 +3058,16 @@
         <v>56</v>
       </c>
       <c r="B59" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="C59" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="D59" t="s">
-        <v>162</v>
+        <v>378</v>
       </c>
       <c r="E59" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -3063,16 +3075,16 @@
         <v>56</v>
       </c>
       <c r="B60" t="s">
-        <v>149</v>
+        <v>187</v>
       </c>
       <c r="C60" t="s">
-        <v>150</v>
+        <v>188</v>
       </c>
       <c r="D60" t="s">
-        <v>380</v>
+        <v>352</v>
       </c>
       <c r="E60" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -3080,16 +3092,16 @@
         <v>56</v>
       </c>
       <c r="B61" t="s">
-        <v>189</v>
+        <v>164</v>
       </c>
       <c r="C61" t="s">
-        <v>190</v>
+        <v>165</v>
       </c>
       <c r="D61" t="s">
-        <v>354</v>
+        <v>166</v>
       </c>
       <c r="E61" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -3097,16 +3109,16 @@
         <v>56</v>
       </c>
       <c r="B62" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C62" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="D62" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="E62" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -3114,16 +3126,16 @@
         <v>56</v>
       </c>
       <c r="B63" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="C63" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="D63" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="E63" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -3131,16 +3143,16 @@
         <v>56</v>
       </c>
       <c r="B64" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C64" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="D64" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="E64" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -3148,16 +3160,16 @@
         <v>56</v>
       </c>
       <c r="B65" t="s">
-        <v>169</v>
+        <v>437</v>
       </c>
       <c r="C65" t="s">
-        <v>170</v>
+        <v>436</v>
       </c>
       <c r="D65" t="s">
-        <v>171</v>
+        <v>420</v>
       </c>
       <c r="E65" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -3165,16 +3177,16 @@
         <v>56</v>
       </c>
       <c r="B66" t="s">
-        <v>439</v>
+        <v>449</v>
       </c>
       <c r="C66" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
       <c r="D66" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="E66" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -3182,16 +3194,16 @@
         <v>56</v>
       </c>
       <c r="B67" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="C67" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="D67" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E67" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -3199,16 +3211,16 @@
         <v>56</v>
       </c>
       <c r="B68" t="s">
-        <v>450</v>
+        <v>442</v>
       </c>
       <c r="C68" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
       <c r="D68" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E68" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -3216,13 +3228,13 @@
         <v>56</v>
       </c>
       <c r="B69" t="s">
-        <v>444</v>
+        <v>204</v>
       </c>
       <c r="C69" t="s">
-        <v>445</v>
+        <v>205</v>
       </c>
       <c r="D69" t="s">
-        <v>425</v>
+        <v>355</v>
       </c>
       <c r="E69" t="s">
         <v>104</v>
@@ -3233,16 +3245,16 @@
         <v>56</v>
       </c>
       <c r="B70" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="C70" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="D70" t="s">
         <v>357</v>
       </c>
       <c r="E70" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -3250,16 +3262,16 @@
         <v>56</v>
       </c>
       <c r="B71" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="C71" t="s">
-        <v>214</v>
+        <v>456</v>
       </c>
       <c r="D71" t="s">
-        <v>359</v>
+        <v>383</v>
       </c>
       <c r="E71" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -3267,16 +3279,16 @@
         <v>56</v>
       </c>
       <c r="B72" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C72" t="s">
-        <v>458</v>
+        <v>465</v>
       </c>
       <c r="D72" t="s">
-        <v>385</v>
+        <v>362</v>
       </c>
       <c r="E72" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -3284,16 +3296,16 @@
         <v>56</v>
       </c>
       <c r="B73" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="C73" t="s">
-        <v>467</v>
+        <v>452</v>
       </c>
       <c r="D73" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="E73" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -3301,16 +3313,16 @@
         <v>56</v>
       </c>
       <c r="B74" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C74" t="s">
-        <v>454</v>
+        <v>464</v>
       </c>
       <c r="D74" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="E74" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -3318,16 +3330,16 @@
         <v>56</v>
       </c>
       <c r="B75" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="C75" t="s">
-        <v>466</v>
+        <v>221</v>
       </c>
       <c r="D75" t="s">
-        <v>358</v>
+        <v>363</v>
       </c>
       <c r="E75" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -3338,13 +3350,13 @@
         <v>222</v>
       </c>
       <c r="C76" t="s">
-        <v>223</v>
+        <v>455</v>
       </c>
       <c r="D76" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E76" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -3352,16 +3364,16 @@
         <v>56</v>
       </c>
       <c r="B77" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C77" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
       <c r="D77" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="E77" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -3369,16 +3381,16 @@
         <v>56</v>
       </c>
       <c r="B78" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C78" t="s">
-        <v>453</v>
+        <v>460</v>
       </c>
       <c r="D78" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E78" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -3386,16 +3398,16 @@
         <v>56</v>
       </c>
       <c r="B79" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="C79" t="s">
-        <v>462</v>
+        <v>453</v>
       </c>
       <c r="D79" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="E79" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -3403,16 +3415,16 @@
         <v>56</v>
       </c>
       <c r="B80" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C80" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="D80" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E80" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -3420,16 +3432,16 @@
         <v>56</v>
       </c>
       <c r="B81" t="s">
-        <v>226</v>
+        <v>203</v>
       </c>
       <c r="C81" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D81" t="s">
-        <v>368</v>
+        <v>354</v>
       </c>
       <c r="E81" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -3437,16 +3449,16 @@
         <v>56</v>
       </c>
       <c r="B82" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C82" t="s">
-        <v>460</v>
+        <v>202</v>
       </c>
       <c r="D82" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="E82" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -3454,16 +3466,16 @@
         <v>56</v>
       </c>
       <c r="B83" t="s">
-        <v>203</v>
+        <v>476</v>
       </c>
       <c r="C83" t="s">
-        <v>204</v>
+        <v>478</v>
       </c>
       <c r="D83" t="s">
-        <v>355</v>
+        <v>480</v>
       </c>
       <c r="E83" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -3471,16 +3483,16 @@
         <v>56</v>
       </c>
       <c r="B84" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C84" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D84" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E84" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -3488,16 +3500,16 @@
         <v>56</v>
       </c>
       <c r="B85" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C85" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D85" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="E85" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -3505,16 +3517,16 @@
         <v>56</v>
       </c>
       <c r="B86" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C86" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D86" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="E86" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -3522,16 +3534,16 @@
         <v>56</v>
       </c>
       <c r="B87" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C87" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D87" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="E87" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -3539,16 +3551,16 @@
         <v>56</v>
       </c>
       <c r="B88" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C88" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D88" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="E88" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -3556,16 +3568,16 @@
         <v>56</v>
       </c>
       <c r="B89" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C89" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="D89" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="E89" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -3573,16 +3585,16 @@
         <v>56</v>
       </c>
       <c r="B90" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C90" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="D90" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="E90" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -3590,16 +3602,16 @@
         <v>56</v>
       </c>
       <c r="B91" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C91" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D91" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="E91" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -3607,16 +3619,16 @@
         <v>56</v>
       </c>
       <c r="B92" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C92" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="D92" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="E92" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -3624,16 +3636,16 @@
         <v>56</v>
       </c>
       <c r="B93" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C93" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="D93" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="E93" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -3641,16 +3653,16 @@
         <v>56</v>
       </c>
       <c r="B94" t="s">
+        <v>475</v>
+      </c>
+      <c r="C94" t="s">
         <v>477</v>
       </c>
-      <c r="C94" t="s">
+      <c r="D94" t="s">
         <v>479</v>
       </c>
-      <c r="D94" t="s">
-        <v>481</v>
-      </c>
       <c r="E94" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -3658,13 +3670,13 @@
         <v>56</v>
       </c>
       <c r="B95" t="s">
-        <v>478</v>
+        <v>259</v>
       </c>
       <c r="C95" t="s">
-        <v>480</v>
+        <v>260</v>
       </c>
       <c r="D95" t="s">
-        <v>482</v>
+        <v>433</v>
       </c>
       <c r="E95" t="s">
         <v>106</v>
@@ -3681,10 +3693,10 @@
         <v>262</v>
       </c>
       <c r="D96" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E96" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -3692,16 +3704,16 @@
         <v>56</v>
       </c>
       <c r="B97" t="s">
-        <v>263</v>
+        <v>299</v>
       </c>
       <c r="C97" t="s">
-        <v>264</v>
+        <v>300</v>
       </c>
       <c r="D97" t="s">
-        <v>436</v>
+        <v>384</v>
       </c>
       <c r="E97" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -3709,16 +3721,16 @@
         <v>56</v>
       </c>
       <c r="B98" t="s">
-        <v>301</v>
+        <v>317</v>
       </c>
       <c r="C98" t="s">
-        <v>302</v>
+        <v>318</v>
       </c>
       <c r="D98" t="s">
-        <v>386</v>
+        <v>319</v>
       </c>
       <c r="E98" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -3726,16 +3738,16 @@
         <v>56</v>
       </c>
       <c r="B99" t="s">
-        <v>319</v>
+        <v>398</v>
       </c>
       <c r="C99" t="s">
-        <v>320</v>
+        <v>234</v>
       </c>
       <c r="D99" t="s">
-        <v>321</v>
+        <v>235</v>
       </c>
       <c r="E99" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -3743,16 +3755,16 @@
         <v>56</v>
       </c>
       <c r="B100" t="s">
-        <v>400</v>
+        <v>428</v>
       </c>
       <c r="C100" t="s">
-        <v>236</v>
+        <v>407</v>
       </c>
       <c r="D100" t="s">
-        <v>237</v>
+        <v>408</v>
       </c>
       <c r="E100" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -3760,16 +3772,16 @@
         <v>56</v>
       </c>
       <c r="B101" t="s">
-        <v>430</v>
+        <v>296</v>
       </c>
       <c r="C101" t="s">
-        <v>409</v>
+        <v>297</v>
       </c>
       <c r="D101" t="s">
-        <v>410</v>
+        <v>298</v>
       </c>
       <c r="E101" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -3777,16 +3789,16 @@
         <v>56</v>
       </c>
       <c r="B102" t="s">
-        <v>298</v>
+        <v>246</v>
       </c>
       <c r="C102" t="s">
-        <v>299</v>
+        <v>247</v>
       </c>
       <c r="D102" t="s">
-        <v>300</v>
+        <v>248</v>
       </c>
       <c r="E102" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -3794,16 +3806,16 @@
         <v>56</v>
       </c>
       <c r="B103" t="s">
-        <v>248</v>
+        <v>228</v>
       </c>
       <c r="C103" t="s">
-        <v>249</v>
+        <v>229</v>
       </c>
       <c r="D103" t="s">
-        <v>250</v>
+        <v>230</v>
       </c>
       <c r="E103" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -3811,16 +3823,16 @@
         <v>56</v>
       </c>
       <c r="B104" t="s">
-        <v>230</v>
+        <v>426</v>
       </c>
       <c r="C104" t="s">
-        <v>231</v>
+        <v>403</v>
       </c>
       <c r="D104" t="s">
-        <v>232</v>
+        <v>404</v>
       </c>
       <c r="E104" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -3828,16 +3840,16 @@
         <v>56</v>
       </c>
       <c r="B105" t="s">
-        <v>428</v>
+        <v>256</v>
       </c>
       <c r="C105" t="s">
-        <v>405</v>
+        <v>257</v>
       </c>
       <c r="D105" t="s">
-        <v>406</v>
+        <v>258</v>
       </c>
       <c r="E105" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -3845,16 +3857,16 @@
         <v>56</v>
       </c>
       <c r="B106" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="C106" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="D106" t="s">
-        <v>260</v>
+        <v>418</v>
       </c>
       <c r="E106" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -3862,16 +3874,16 @@
         <v>56</v>
       </c>
       <c r="B107" t="s">
-        <v>265</v>
+        <v>432</v>
       </c>
       <c r="C107" t="s">
-        <v>266</v>
+        <v>413</v>
       </c>
       <c r="D107" t="s">
-        <v>420</v>
+        <v>435</v>
       </c>
       <c r="E107" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -3879,16 +3891,16 @@
         <v>56</v>
       </c>
       <c r="B108" t="s">
-        <v>434</v>
+        <v>254</v>
       </c>
       <c r="C108" t="s">
-        <v>415</v>
+        <v>255</v>
       </c>
       <c r="D108" t="s">
-        <v>437</v>
+        <v>388</v>
       </c>
       <c r="E108" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -3896,16 +3908,16 @@
         <v>56</v>
       </c>
       <c r="B109" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="C109" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="D109" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="E109" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
@@ -3913,16 +3925,16 @@
         <v>56</v>
       </c>
       <c r="B110" t="s">
-        <v>251</v>
+        <v>307</v>
       </c>
       <c r="C110" t="s">
-        <v>252</v>
+        <v>308</v>
       </c>
       <c r="D110" t="s">
-        <v>389</v>
+        <v>309</v>
       </c>
       <c r="E110" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -3930,16 +3942,16 @@
         <v>56</v>
       </c>
       <c r="B111" t="s">
-        <v>309</v>
+        <v>243</v>
       </c>
       <c r="C111" t="s">
-        <v>310</v>
+        <v>244</v>
       </c>
       <c r="D111" t="s">
-        <v>311</v>
+        <v>245</v>
       </c>
       <c r="E111" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -3947,16 +3959,16 @@
         <v>56</v>
       </c>
       <c r="B112" t="s">
-        <v>245</v>
+        <v>290</v>
       </c>
       <c r="C112" t="s">
-        <v>246</v>
+        <v>291</v>
       </c>
       <c r="D112" t="s">
-        <v>247</v>
+        <v>292</v>
       </c>
       <c r="E112" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -3964,16 +3976,16 @@
         <v>56</v>
       </c>
       <c r="B113" t="s">
-        <v>292</v>
+        <v>231</v>
       </c>
       <c r="C113" t="s">
-        <v>293</v>
+        <v>232</v>
       </c>
       <c r="D113" t="s">
-        <v>294</v>
+        <v>233</v>
       </c>
       <c r="E113" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -3981,16 +3993,16 @@
         <v>56</v>
       </c>
       <c r="B114" t="s">
-        <v>233</v>
+        <v>427</v>
       </c>
       <c r="C114" t="s">
-        <v>234</v>
+        <v>405</v>
       </c>
       <c r="D114" t="s">
-        <v>235</v>
+        <v>406</v>
       </c>
       <c r="E114" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -3998,16 +4010,16 @@
         <v>56</v>
       </c>
       <c r="B115" t="s">
-        <v>429</v>
+        <v>293</v>
       </c>
       <c r="C115" t="s">
-        <v>407</v>
+        <v>294</v>
       </c>
       <c r="D115" t="s">
-        <v>408</v>
+        <v>295</v>
       </c>
       <c r="E115" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
@@ -4015,16 +4027,16 @@
         <v>56</v>
       </c>
       <c r="B116" t="s">
-        <v>295</v>
+        <v>320</v>
       </c>
       <c r="C116" t="s">
-        <v>296</v>
+        <v>321</v>
       </c>
       <c r="D116" t="s">
-        <v>297</v>
+        <v>322</v>
       </c>
       <c r="E116" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
@@ -4032,16 +4044,16 @@
         <v>56</v>
       </c>
       <c r="B117" t="s">
-        <v>322</v>
+        <v>239</v>
       </c>
       <c r="C117" t="s">
-        <v>323</v>
+        <v>240</v>
       </c>
       <c r="D117" t="s">
-        <v>324</v>
+        <v>416</v>
       </c>
       <c r="E117" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -4049,16 +4061,16 @@
         <v>56</v>
       </c>
       <c r="B118" t="s">
-        <v>241</v>
+        <v>430</v>
       </c>
       <c r="C118" t="s">
-        <v>242</v>
+        <v>411</v>
       </c>
       <c r="D118" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="E118" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
@@ -4066,16 +4078,16 @@
         <v>56</v>
       </c>
       <c r="B119" t="s">
-        <v>432</v>
+        <v>278</v>
       </c>
       <c r="C119" t="s">
-        <v>413</v>
+        <v>279</v>
       </c>
       <c r="D119" t="s">
-        <v>416</v>
+        <v>280</v>
       </c>
       <c r="E119" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
@@ -4083,16 +4095,16 @@
         <v>56</v>
       </c>
       <c r="B120" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C120" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D120" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E120" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
@@ -4100,16 +4112,16 @@
         <v>56</v>
       </c>
       <c r="B121" t="s">
+        <v>284</v>
+      </c>
+      <c r="C121" t="s">
+        <v>285</v>
+      </c>
+      <c r="D121" t="s">
         <v>286</v>
       </c>
-      <c r="C121" t="s">
-        <v>287</v>
-      </c>
-      <c r="D121" t="s">
-        <v>288</v>
-      </c>
       <c r="E121" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
@@ -4117,16 +4129,16 @@
         <v>56</v>
       </c>
       <c r="B122" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="C122" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="D122" t="s">
-        <v>285</v>
+        <v>370</v>
       </c>
       <c r="E122" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
@@ -4140,10 +4152,10 @@
         <v>277</v>
       </c>
       <c r="D123" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E123" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
@@ -4151,16 +4163,16 @@
         <v>56</v>
       </c>
       <c r="B124" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
       <c r="C124" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
       <c r="D124" t="s">
-        <v>373</v>
+        <v>419</v>
       </c>
       <c r="E124" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
@@ -4174,10 +4186,10 @@
         <v>268</v>
       </c>
       <c r="D125" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="E125" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
@@ -4185,16 +4197,16 @@
         <v>56</v>
       </c>
       <c r="B126" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C126" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D126" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="E126" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
@@ -4202,16 +4214,16 @@
         <v>56</v>
       </c>
       <c r="B127" t="s">
-        <v>269</v>
+        <v>287</v>
       </c>
       <c r="C127" t="s">
-        <v>270</v>
+        <v>288</v>
       </c>
       <c r="D127" t="s">
-        <v>426</v>
+        <v>289</v>
       </c>
       <c r="E127" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
@@ -4219,16 +4231,16 @@
         <v>56</v>
       </c>
       <c r="B128" t="s">
-        <v>289</v>
+        <v>236</v>
       </c>
       <c r="C128" t="s">
-        <v>290</v>
+        <v>237</v>
       </c>
       <c r="D128" t="s">
-        <v>291</v>
+        <v>238</v>
       </c>
       <c r="E128" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
@@ -4236,16 +4248,16 @@
         <v>56</v>
       </c>
       <c r="B129" t="s">
-        <v>238</v>
+        <v>429</v>
       </c>
       <c r="C129" t="s">
-        <v>239</v>
+        <v>409</v>
       </c>
       <c r="D129" t="s">
-        <v>240</v>
+        <v>410</v>
       </c>
       <c r="E129" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
@@ -4253,16 +4265,16 @@
         <v>56</v>
       </c>
       <c r="B130" t="s">
-        <v>431</v>
+        <v>271</v>
       </c>
       <c r="C130" t="s">
-        <v>411</v>
+        <v>272</v>
       </c>
       <c r="D130" t="s">
-        <v>412</v>
+        <v>273</v>
       </c>
       <c r="E130" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
@@ -4270,16 +4282,16 @@
         <v>56</v>
       </c>
       <c r="B131" t="s">
-        <v>273</v>
+        <v>301</v>
       </c>
       <c r="C131" t="s">
-        <v>274</v>
+        <v>302</v>
       </c>
       <c r="D131" t="s">
-        <v>275</v>
+        <v>303</v>
       </c>
       <c r="E131" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
@@ -4287,16 +4299,16 @@
         <v>56</v>
       </c>
       <c r="B132" t="s">
-        <v>303</v>
+        <v>316</v>
       </c>
       <c r="C132" t="s">
-        <v>304</v>
+        <v>402</v>
       </c>
       <c r="D132" t="s">
-        <v>305</v>
+        <v>401</v>
       </c>
       <c r="E132" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
@@ -4304,16 +4316,16 @@
         <v>56</v>
       </c>
       <c r="B133" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="C133" t="s">
-        <v>404</v>
+        <v>314</v>
       </c>
       <c r="D133" t="s">
-        <v>403</v>
+        <v>315</v>
       </c>
       <c r="E133" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
@@ -4321,16 +4333,16 @@
         <v>56</v>
       </c>
       <c r="B134" t="s">
-        <v>315</v>
+        <v>251</v>
       </c>
       <c r="C134" t="s">
-        <v>316</v>
+        <v>252</v>
       </c>
       <c r="D134" t="s">
-        <v>317</v>
+        <v>253</v>
       </c>
       <c r="E134" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
@@ -4338,16 +4350,16 @@
         <v>56</v>
       </c>
       <c r="B135" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="C135" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
       <c r="D135" t="s">
-        <v>255</v>
+        <v>417</v>
       </c>
       <c r="E135" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
@@ -4355,16 +4367,16 @@
         <v>56</v>
       </c>
       <c r="B136" t="s">
-        <v>243</v>
+        <v>431</v>
       </c>
       <c r="C136" t="s">
-        <v>244</v>
+        <v>412</v>
       </c>
       <c r="D136" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="E136" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
@@ -4372,16 +4384,16 @@
         <v>56</v>
       </c>
       <c r="B137" t="s">
-        <v>433</v>
+        <v>310</v>
       </c>
       <c r="C137" t="s">
-        <v>414</v>
+        <v>311</v>
       </c>
       <c r="D137" t="s">
-        <v>417</v>
+        <v>312</v>
       </c>
       <c r="E137" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
@@ -4389,16 +4401,16 @@
         <v>56</v>
       </c>
       <c r="B138" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="C138" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="D138" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="E138" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
@@ -4406,38 +4418,21 @@
         <v>56</v>
       </c>
       <c r="B139" t="s">
-        <v>306</v>
+        <v>399</v>
       </c>
       <c r="C139" t="s">
-        <v>307</v>
+        <v>400</v>
       </c>
       <c r="D139" t="s">
-        <v>308</v>
+        <v>386</v>
       </c>
       <c r="E139" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>56</v>
-      </c>
-      <c r="B140" t="s">
-        <v>401</v>
-      </c>
-      <c r="C140" t="s">
-        <v>402</v>
-      </c>
-      <c r="D140" t="s">
-        <v>388</v>
-      </c>
-      <c r="E140" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A96:E140">
-    <sortCondition ref="C96:C140"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A95:E139">
+    <sortCondition ref="C95:C139"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -4463,33 +4458,33 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>323</v>
+      </c>
+      <c r="B1" t="s">
+        <v>324</v>
+      </c>
+      <c r="C1" t="s">
         <v>325</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>326</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>327</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>328</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>329</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>330</v>
-      </c>
-      <c r="G1" t="s">
-        <v>331</v>
-      </c>
-      <c r="H1" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B2" t="s">
         <v>22</v>
@@ -4504,10 +4499,10 @@
         <v>56</v>
       </c>
       <c r="F2" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="G2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="H2" t="s">
         <v>54</v>

</xml_diff>

<commit_message>
Fix icon settings updates
</commit_message>
<xml_diff>
--- a/form.xlsx
+++ b/form.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\aerialsurvey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9894638-CF30-4B92-968A-F48D885F155A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{150810AD-0547-4918-8D86-04BFD2A44DCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11205" yWindow="0" windowWidth="35190" windowHeight="20985" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11550" yWindow="1890" windowWidth="35190" windowHeight="12690" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="479">
   <si>
     <t>type</t>
   </si>
@@ -264,12 +264,6 @@
     <t>Falk</t>
   </si>
   <si>
-    <t>richard</t>
-  </si>
-  <si>
-    <t>Richard</t>
-  </si>
-  <si>
     <t>recce</t>
   </si>
   <si>
@@ -1443,12 +1437,6 @@
     <t>Birds.svg</t>
   </si>
   <si>
-    <t>Aaron Nicholas</t>
-  </si>
-  <si>
-    <t>aaron_nicholas</t>
-  </si>
-  <si>
     <t>vulture_nest</t>
   </si>
   <si>
@@ -1465,6 +1453,12 @@
   </si>
   <si>
     <t>Ostrich nest.svg</t>
+  </si>
+  <si>
+    <t>Aaron</t>
+  </si>
+  <si>
+    <t>aaron</t>
   </si>
 </sst>
 </file>
@@ -1850,7 +1844,7 @@
         <v>9</v>
       </c>
       <c r="F1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
@@ -1859,7 +1853,7 @@
         <v>5</v>
       </c>
       <c r="I1" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="J1" t="s">
         <v>6</v>
@@ -1891,10 +1885,10 @@
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D2" t="s">
         <v>15</v>
@@ -1931,7 +1925,7 @@
         <v>22</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="J4" t="s">
         <v>23</v>
@@ -1968,7 +1962,7 @@
         <v>29</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="J6" t="s">
         <v>23</v>
@@ -2013,16 +2007,16 @@
         <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C9" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E9" t="s">
         <v>23</v>
       </c>
       <c r="F9" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -2044,13 +2038,13 @@
         <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C11" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="F11" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -2072,13 +2066,13 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
+        <v>336</v>
+      </c>
+      <c r="C13" t="s">
         <v>338</v>
       </c>
-      <c r="C13" t="s">
-        <v>340</v>
-      </c>
       <c r="F13" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -2100,13 +2094,13 @@
         <v>20</v>
       </c>
       <c r="B15" t="s">
+        <v>337</v>
+      </c>
+      <c r="C15" t="s">
         <v>339</v>
       </c>
-      <c r="C15" t="s">
-        <v>341</v>
-      </c>
       <c r="F15" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
@@ -2165,7 +2159,7 @@
         <v>35</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="J19" t="s">
         <v>23</v>
@@ -2266,10 +2260,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E139"/>
+  <dimension ref="A1:E138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A82" sqref="A82"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2302,10 +2296,10 @@
         <v>73</v>
       </c>
       <c r="B2" t="s">
-        <v>474</v>
+        <v>478</v>
       </c>
       <c r="C2" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2346,21 +2340,21 @@
         <v>73</v>
       </c>
       <c r="B6" t="s">
+        <v>332</v>
+      </c>
+      <c r="C6" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" t="s">
         <v>80</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C8" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>73</v>
-      </c>
-      <c r="B7" t="s">
-        <v>334</v>
-      </c>
-      <c r="C7" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -2396,14 +2390,14 @@
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" t="s">
         <v>88</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2412,21 +2406,21 @@
         <v>60</v>
       </c>
       <c r="B14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" t="s">
         <v>90</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C16" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>60</v>
-      </c>
-      <c r="B15" t="s">
-        <v>63</v>
-      </c>
-      <c r="C15" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -2440,14 +2434,14 @@
         <v>93</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>66</v>
-      </c>
-      <c r="B18" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" t="s">
         <v>94</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>95</v>
       </c>
     </row>
@@ -2473,15 +2467,18 @@
         <v>99</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>69</v>
-      </c>
-      <c r="B22" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" t="s">
         <v>100</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>101</v>
+      </c>
+      <c r="D23" t="s">
+        <v>468</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -2506,24 +2503,27 @@
         <v>104</v>
       </c>
       <c r="C25" t="s">
-        <v>105</v>
+        <v>395</v>
       </c>
       <c r="D25" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>50</v>
-      </c>
-      <c r="B26" t="s">
-        <v>106</v>
-      </c>
-      <c r="C26" t="s">
-        <v>397</v>
-      </c>
-      <c r="D26" t="s">
-        <v>471</v>
+        <v>469</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" t="s">
+        <v>437</v>
+      </c>
+      <c r="C27" t="s">
+        <v>438</v>
+      </c>
+      <c r="D27" t="s">
+        <v>387</v>
+      </c>
+      <c r="E27" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -2531,16 +2531,16 @@
         <v>56</v>
       </c>
       <c r="B28" t="s">
-        <v>439</v>
+        <v>184</v>
       </c>
       <c r="C28" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="D28" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E28" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -2548,16 +2548,16 @@
         <v>56</v>
       </c>
       <c r="B29" t="s">
-        <v>186</v>
+        <v>111</v>
       </c>
       <c r="C29" t="s">
-        <v>444</v>
+        <v>112</v>
       </c>
       <c r="D29" t="s">
-        <v>390</v>
+        <v>113</v>
       </c>
       <c r="E29" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -2565,16 +2565,16 @@
         <v>56</v>
       </c>
       <c r="B30" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="C30" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="D30" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E30" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -2582,16 +2582,16 @@
         <v>56</v>
       </c>
       <c r="B31" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C31" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D31" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E31" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -2599,16 +2599,16 @@
         <v>56</v>
       </c>
       <c r="B32" t="s">
-        <v>110</v>
+        <v>174</v>
       </c>
       <c r="C32" t="s">
-        <v>111</v>
+        <v>175</v>
       </c>
       <c r="D32" t="s">
-        <v>112</v>
+        <v>176</v>
       </c>
       <c r="E32" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -2616,16 +2616,16 @@
         <v>56</v>
       </c>
       <c r="B33" t="s">
-        <v>176</v>
+        <v>114</v>
       </c>
       <c r="C33" t="s">
-        <v>177</v>
+        <v>115</v>
       </c>
       <c r="D33" t="s">
-        <v>178</v>
+        <v>116</v>
       </c>
       <c r="E33" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -2633,16 +2633,16 @@
         <v>56</v>
       </c>
       <c r="B34" t="s">
-        <v>116</v>
+        <v>187</v>
       </c>
       <c r="C34" t="s">
-        <v>117</v>
+        <v>188</v>
       </c>
       <c r="D34" t="s">
-        <v>118</v>
+        <v>189</v>
       </c>
       <c r="E34" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -2650,16 +2650,16 @@
         <v>56</v>
       </c>
       <c r="B35" t="s">
-        <v>189</v>
+        <v>117</v>
       </c>
       <c r="C35" t="s">
-        <v>190</v>
+        <v>118</v>
       </c>
       <c r="D35" t="s">
-        <v>191</v>
+        <v>349</v>
       </c>
       <c r="E35" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -2673,10 +2673,10 @@
         <v>120</v>
       </c>
       <c r="D36" t="s">
-        <v>351</v>
+        <v>121</v>
       </c>
       <c r="E36" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -2684,16 +2684,16 @@
         <v>56</v>
       </c>
       <c r="B37" t="s">
-        <v>121</v>
+        <v>196</v>
       </c>
       <c r="C37" t="s">
-        <v>122</v>
+        <v>197</v>
       </c>
       <c r="D37" t="s">
-        <v>123</v>
+        <v>198</v>
       </c>
       <c r="E37" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -2701,16 +2701,16 @@
         <v>56</v>
       </c>
       <c r="B38" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="C38" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="D38" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="E38" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -2718,16 +2718,16 @@
         <v>56</v>
       </c>
       <c r="B39" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C39" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="D39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="E39" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -2735,16 +2735,16 @@
         <v>56</v>
       </c>
       <c r="B40" t="s">
-        <v>192</v>
+        <v>125</v>
       </c>
       <c r="C40" t="s">
-        <v>193</v>
+        <v>126</v>
       </c>
       <c r="D40" t="s">
-        <v>194</v>
+        <v>127</v>
       </c>
       <c r="E40" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -2752,16 +2752,16 @@
         <v>56</v>
       </c>
       <c r="B41" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C41" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D41" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E41" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -2769,16 +2769,16 @@
         <v>56</v>
       </c>
       <c r="B42" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C42" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="D42" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="E42" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -2786,16 +2786,16 @@
         <v>56</v>
       </c>
       <c r="B43" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C43" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D43" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E43" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -2803,16 +2803,16 @@
         <v>56</v>
       </c>
       <c r="B44" t="s">
-        <v>133</v>
+        <v>182</v>
       </c>
       <c r="C44" t="s">
-        <v>134</v>
+        <v>443</v>
       </c>
       <c r="D44" t="s">
-        <v>135</v>
+        <v>183</v>
       </c>
       <c r="E44" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -2820,16 +2820,16 @@
         <v>56</v>
       </c>
       <c r="B45" t="s">
-        <v>184</v>
+        <v>153</v>
       </c>
       <c r="C45" t="s">
-        <v>445</v>
+        <v>154</v>
       </c>
       <c r="D45" t="s">
-        <v>185</v>
+        <v>155</v>
       </c>
       <c r="E45" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -2837,16 +2837,16 @@
         <v>56</v>
       </c>
       <c r="B46" t="s">
-        <v>155</v>
+        <v>180</v>
       </c>
       <c r="C46" t="s">
-        <v>156</v>
+        <v>181</v>
       </c>
       <c r="D46" t="s">
-        <v>157</v>
+        <v>375</v>
       </c>
       <c r="E46" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -2854,16 +2854,16 @@
         <v>56</v>
       </c>
       <c r="B47" t="s">
-        <v>182</v>
+        <v>134</v>
       </c>
       <c r="C47" t="s">
-        <v>183</v>
+        <v>135</v>
       </c>
       <c r="D47" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
       <c r="E47" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -2871,16 +2871,16 @@
         <v>56</v>
       </c>
       <c r="B48" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C48" t="s">
-        <v>137</v>
+        <v>445</v>
       </c>
       <c r="D48" t="s">
-        <v>372</v>
+        <v>139</v>
       </c>
       <c r="E48" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -2888,16 +2888,16 @@
         <v>56</v>
       </c>
       <c r="B49" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C49" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="D49" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E49" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -2905,16 +2905,16 @@
         <v>56</v>
       </c>
       <c r="B50" t="s">
-        <v>138</v>
+        <v>177</v>
       </c>
       <c r="C50" t="s">
-        <v>446</v>
+        <v>178</v>
       </c>
       <c r="D50" t="s">
-        <v>139</v>
+        <v>179</v>
       </c>
       <c r="E50" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -2922,16 +2922,16 @@
         <v>56</v>
       </c>
       <c r="B51" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="C51" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="D51" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="E51" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -2939,16 +2939,16 @@
         <v>56</v>
       </c>
       <c r="B52" t="s">
-        <v>173</v>
+        <v>142</v>
       </c>
       <c r="C52" t="s">
-        <v>174</v>
+        <v>143</v>
       </c>
       <c r="D52" t="s">
-        <v>175</v>
+        <v>144</v>
       </c>
       <c r="E52" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -2956,16 +2956,16 @@
         <v>56</v>
       </c>
       <c r="B53" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C53" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D53" t="s">
-        <v>146</v>
+        <v>374</v>
       </c>
       <c r="E53" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -2973,16 +2973,16 @@
         <v>56</v>
       </c>
       <c r="B54" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="C54" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="D54" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="E54" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -2996,10 +2996,10 @@
         <v>150</v>
       </c>
       <c r="D55" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E55" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -3013,10 +3013,10 @@
         <v>152</v>
       </c>
       <c r="D56" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E56" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -3024,16 +3024,16 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C57" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="D57" t="s">
-        <v>375</v>
+        <v>158</v>
       </c>
       <c r="E57" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -3041,16 +3041,16 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="C58" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="D58" t="s">
-        <v>160</v>
+        <v>376</v>
       </c>
       <c r="E58" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -3058,16 +3058,16 @@
         <v>56</v>
       </c>
       <c r="B59" t="s">
-        <v>147</v>
+        <v>185</v>
       </c>
       <c r="C59" t="s">
-        <v>148</v>
+        <v>186</v>
       </c>
       <c r="D59" t="s">
-        <v>378</v>
+        <v>350</v>
       </c>
       <c r="E59" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -3075,16 +3075,16 @@
         <v>56</v>
       </c>
       <c r="B60" t="s">
-        <v>187</v>
+        <v>162</v>
       </c>
       <c r="C60" t="s">
-        <v>188</v>
+        <v>163</v>
       </c>
       <c r="D60" t="s">
-        <v>352</v>
+        <v>164</v>
       </c>
       <c r="E60" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -3092,16 +3092,16 @@
         <v>56</v>
       </c>
       <c r="B61" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="C61" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D61" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="E61" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -3109,16 +3109,16 @@
         <v>56</v>
       </c>
       <c r="B62" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="C62" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="D62" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="E62" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -3126,16 +3126,16 @@
         <v>56</v>
       </c>
       <c r="B63" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C63" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D63" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E63" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -3143,16 +3143,16 @@
         <v>56</v>
       </c>
       <c r="B64" t="s">
-        <v>167</v>
+        <v>435</v>
       </c>
       <c r="C64" t="s">
-        <v>168</v>
+        <v>434</v>
       </c>
       <c r="D64" t="s">
-        <v>169</v>
+        <v>418</v>
       </c>
       <c r="E64" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -3160,16 +3160,16 @@
         <v>56</v>
       </c>
       <c r="B65" t="s">
-        <v>437</v>
+        <v>447</v>
       </c>
       <c r="C65" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
       <c r="D65" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E65" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -3177,16 +3177,16 @@
         <v>56</v>
       </c>
       <c r="B66" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="C66" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="D66" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E66" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -3194,16 +3194,16 @@
         <v>56</v>
       </c>
       <c r="B67" t="s">
-        <v>448</v>
+        <v>440</v>
       </c>
       <c r="C67" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
       <c r="D67" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="E67" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -3211,13 +3211,13 @@
         <v>56</v>
       </c>
       <c r="B68" t="s">
-        <v>442</v>
+        <v>202</v>
       </c>
       <c r="C68" t="s">
-        <v>443</v>
+        <v>203</v>
       </c>
       <c r="D68" t="s">
-        <v>423</v>
+        <v>353</v>
       </c>
       <c r="E68" t="s">
         <v>102</v>
@@ -3228,16 +3228,16 @@
         <v>56</v>
       </c>
       <c r="B69" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="C69" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="D69" t="s">
         <v>355</v>
       </c>
       <c r="E69" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -3245,16 +3245,16 @@
         <v>56</v>
       </c>
       <c r="B70" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C70" t="s">
-        <v>212</v>
+        <v>454</v>
       </c>
       <c r="D70" t="s">
-        <v>357</v>
+        <v>381</v>
       </c>
       <c r="E70" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -3262,16 +3262,16 @@
         <v>56</v>
       </c>
       <c r="B71" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C71" t="s">
-        <v>456</v>
+        <v>463</v>
       </c>
       <c r="D71" t="s">
-        <v>383</v>
+        <v>360</v>
       </c>
       <c r="E71" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -3279,16 +3279,16 @@
         <v>56</v>
       </c>
       <c r="B72" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="C72" t="s">
-        <v>465</v>
+        <v>450</v>
       </c>
       <c r="D72" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="E72" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -3296,16 +3296,16 @@
         <v>56</v>
       </c>
       <c r="B73" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="C73" t="s">
-        <v>452</v>
+        <v>462</v>
       </c>
       <c r="D73" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="E73" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -3313,16 +3313,16 @@
         <v>56</v>
       </c>
       <c r="B74" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="C74" t="s">
-        <v>464</v>
+        <v>219</v>
       </c>
       <c r="D74" t="s">
-        <v>356</v>
+        <v>361</v>
       </c>
       <c r="E74" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -3333,13 +3333,13 @@
         <v>220</v>
       </c>
       <c r="C75" t="s">
-        <v>221</v>
+        <v>453</v>
       </c>
       <c r="D75" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E75" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -3347,16 +3347,16 @@
         <v>56</v>
       </c>
       <c r="B76" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C76" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
       <c r="D76" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="E76" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -3364,16 +3364,16 @@
         <v>56</v>
       </c>
       <c r="B77" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C77" t="s">
-        <v>451</v>
+        <v>458</v>
       </c>
       <c r="D77" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E77" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -3381,16 +3381,16 @@
         <v>56</v>
       </c>
       <c r="B78" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="C78" t="s">
-        <v>460</v>
+        <v>451</v>
       </c>
       <c r="D78" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="E78" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -3398,16 +3398,16 @@
         <v>56</v>
       </c>
       <c r="B79" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C79" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="D79" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E79" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -3415,16 +3415,16 @@
         <v>56</v>
       </c>
       <c r="B80" t="s">
-        <v>224</v>
+        <v>201</v>
       </c>
       <c r="C80" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D80" t="s">
-        <v>366</v>
+        <v>352</v>
       </c>
       <c r="E80" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -3432,16 +3432,16 @@
         <v>56</v>
       </c>
       <c r="B81" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C81" t="s">
-        <v>458</v>
+        <v>200</v>
       </c>
       <c r="D81" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="E81" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -3449,16 +3449,16 @@
         <v>56</v>
       </c>
       <c r="B82" t="s">
-        <v>201</v>
+        <v>472</v>
       </c>
       <c r="C82" t="s">
-        <v>202</v>
+        <v>474</v>
       </c>
       <c r="D82" t="s">
-        <v>353</v>
+        <v>476</v>
       </c>
       <c r="E82" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -3466,16 +3466,16 @@
         <v>56</v>
       </c>
       <c r="B83" t="s">
-        <v>476</v>
+        <v>225</v>
       </c>
       <c r="C83" t="s">
-        <v>478</v>
+        <v>452</v>
       </c>
       <c r="D83" t="s">
-        <v>480</v>
+        <v>367</v>
       </c>
       <c r="E83" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -3483,16 +3483,16 @@
         <v>56</v>
       </c>
       <c r="B84" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="C84" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
       <c r="D84" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
       <c r="E84" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -3500,16 +3500,16 @@
         <v>56</v>
       </c>
       <c r="B85" t="s">
-        <v>217</v>
+        <v>393</v>
       </c>
       <c r="C85" t="s">
-        <v>450</v>
+        <v>460</v>
       </c>
       <c r="D85" t="s">
-        <v>361</v>
+        <v>394</v>
       </c>
       <c r="E85" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -3517,16 +3517,16 @@
         <v>56</v>
       </c>
       <c r="B86" t="s">
-        <v>395</v>
+        <v>213</v>
       </c>
       <c r="C86" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D86" t="s">
-        <v>396</v>
+        <v>383</v>
       </c>
       <c r="E86" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -3534,16 +3534,16 @@
         <v>56</v>
       </c>
       <c r="B87" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C87" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
       <c r="D87" t="s">
-        <v>385</v>
+        <v>358</v>
       </c>
       <c r="E87" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -3551,16 +3551,16 @@
         <v>56</v>
       </c>
       <c r="B88" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C88" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D88" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="E88" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -3568,16 +3568,16 @@
         <v>56</v>
       </c>
       <c r="B89" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="C89" t="s">
-        <v>469</v>
+        <v>457</v>
       </c>
       <c r="D89" t="s">
-        <v>359</v>
+        <v>378</v>
       </c>
       <c r="E89" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -3585,16 +3585,16 @@
         <v>56</v>
       </c>
       <c r="B90" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C90" t="s">
         <v>459</v>
       </c>
       <c r="D90" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E90" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -3602,16 +3602,16 @@
         <v>56</v>
       </c>
       <c r="B91" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C91" t="s">
-        <v>461</v>
+        <v>464</v>
       </c>
       <c r="D91" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="E91" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -3619,16 +3619,16 @@
         <v>56</v>
       </c>
       <c r="B92" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C92" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D92" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="E92" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -3636,16 +3636,16 @@
         <v>56</v>
       </c>
       <c r="B93" t="s">
-        <v>209</v>
+        <v>471</v>
       </c>
       <c r="C93" t="s">
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="D93" t="s">
-        <v>382</v>
+        <v>475</v>
       </c>
       <c r="E93" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -3653,13 +3653,13 @@
         <v>56</v>
       </c>
       <c r="B94" t="s">
-        <v>475</v>
+        <v>257</v>
       </c>
       <c r="C94" t="s">
-        <v>477</v>
+        <v>258</v>
       </c>
       <c r="D94" t="s">
-        <v>479</v>
+        <v>431</v>
       </c>
       <c r="E94" t="s">
         <v>104</v>
@@ -3676,10 +3676,10 @@
         <v>260</v>
       </c>
       <c r="D95" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E95" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -3687,16 +3687,16 @@
         <v>56</v>
       </c>
       <c r="B96" t="s">
-        <v>261</v>
+        <v>297</v>
       </c>
       <c r="C96" t="s">
-        <v>262</v>
+        <v>298</v>
       </c>
       <c r="D96" t="s">
-        <v>434</v>
+        <v>382</v>
       </c>
       <c r="E96" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -3704,16 +3704,16 @@
         <v>56</v>
       </c>
       <c r="B97" t="s">
-        <v>299</v>
+        <v>315</v>
       </c>
       <c r="C97" t="s">
-        <v>300</v>
+        <v>316</v>
       </c>
       <c r="D97" t="s">
-        <v>384</v>
+        <v>317</v>
       </c>
       <c r="E97" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -3721,16 +3721,16 @@
         <v>56</v>
       </c>
       <c r="B98" t="s">
-        <v>317</v>
+        <v>396</v>
       </c>
       <c r="C98" t="s">
-        <v>318</v>
+        <v>232</v>
       </c>
       <c r="D98" t="s">
-        <v>319</v>
+        <v>233</v>
       </c>
       <c r="E98" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -3738,16 +3738,16 @@
         <v>56</v>
       </c>
       <c r="B99" t="s">
-        <v>398</v>
+        <v>426</v>
       </c>
       <c r="C99" t="s">
-        <v>234</v>
+        <v>405</v>
       </c>
       <c r="D99" t="s">
-        <v>235</v>
+        <v>406</v>
       </c>
       <c r="E99" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -3755,16 +3755,16 @@
         <v>56</v>
       </c>
       <c r="B100" t="s">
-        <v>428</v>
+        <v>294</v>
       </c>
       <c r="C100" t="s">
-        <v>407</v>
+        <v>295</v>
       </c>
       <c r="D100" t="s">
-        <v>408</v>
+        <v>296</v>
       </c>
       <c r="E100" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -3772,16 +3772,16 @@
         <v>56</v>
       </c>
       <c r="B101" t="s">
-        <v>296</v>
+        <v>244</v>
       </c>
       <c r="C101" t="s">
-        <v>297</v>
+        <v>245</v>
       </c>
       <c r="D101" t="s">
-        <v>298</v>
+        <v>246</v>
       </c>
       <c r="E101" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -3789,16 +3789,16 @@
         <v>56</v>
       </c>
       <c r="B102" t="s">
-        <v>246</v>
+        <v>226</v>
       </c>
       <c r="C102" t="s">
-        <v>247</v>
+        <v>227</v>
       </c>
       <c r="D102" t="s">
-        <v>248</v>
+        <v>228</v>
       </c>
       <c r="E102" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -3806,16 +3806,16 @@
         <v>56</v>
       </c>
       <c r="B103" t="s">
-        <v>228</v>
+        <v>424</v>
       </c>
       <c r="C103" t="s">
-        <v>229</v>
+        <v>401</v>
       </c>
       <c r="D103" t="s">
-        <v>230</v>
+        <v>402</v>
       </c>
       <c r="E103" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -3823,16 +3823,16 @@
         <v>56</v>
       </c>
       <c r="B104" t="s">
-        <v>426</v>
+        <v>254</v>
       </c>
       <c r="C104" t="s">
-        <v>403</v>
+        <v>255</v>
       </c>
       <c r="D104" t="s">
-        <v>404</v>
+        <v>256</v>
       </c>
       <c r="E104" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -3840,16 +3840,16 @@
         <v>56</v>
       </c>
       <c r="B105" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="C105" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="D105" t="s">
-        <v>258</v>
+        <v>416</v>
       </c>
       <c r="E105" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -3857,16 +3857,16 @@
         <v>56</v>
       </c>
       <c r="B106" t="s">
-        <v>263</v>
+        <v>430</v>
       </c>
       <c r="C106" t="s">
-        <v>264</v>
+        <v>411</v>
       </c>
       <c r="D106" t="s">
-        <v>418</v>
+        <v>433</v>
       </c>
       <c r="E106" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -3874,16 +3874,16 @@
         <v>56</v>
       </c>
       <c r="B107" t="s">
-        <v>432</v>
+        <v>252</v>
       </c>
       <c r="C107" t="s">
-        <v>413</v>
+        <v>253</v>
       </c>
       <c r="D107" t="s">
-        <v>435</v>
+        <v>386</v>
       </c>
       <c r="E107" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -3891,16 +3891,16 @@
         <v>56</v>
       </c>
       <c r="B108" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="C108" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="D108" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="E108" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -3908,16 +3908,16 @@
         <v>56</v>
       </c>
       <c r="B109" t="s">
-        <v>249</v>
+        <v>305</v>
       </c>
       <c r="C109" t="s">
-        <v>250</v>
+        <v>306</v>
       </c>
       <c r="D109" t="s">
-        <v>387</v>
+        <v>307</v>
       </c>
       <c r="E109" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
@@ -3925,16 +3925,16 @@
         <v>56</v>
       </c>
       <c r="B110" t="s">
-        <v>307</v>
+        <v>241</v>
       </c>
       <c r="C110" t="s">
-        <v>308</v>
+        <v>242</v>
       </c>
       <c r="D110" t="s">
-        <v>309</v>
+        <v>243</v>
       </c>
       <c r="E110" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -3942,16 +3942,16 @@
         <v>56</v>
       </c>
       <c r="B111" t="s">
-        <v>243</v>
+        <v>288</v>
       </c>
       <c r="C111" t="s">
-        <v>244</v>
+        <v>289</v>
       </c>
       <c r="D111" t="s">
-        <v>245</v>
+        <v>290</v>
       </c>
       <c r="E111" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -3959,16 +3959,16 @@
         <v>56</v>
       </c>
       <c r="B112" t="s">
-        <v>290</v>
+        <v>229</v>
       </c>
       <c r="C112" t="s">
-        <v>291</v>
+        <v>230</v>
       </c>
       <c r="D112" t="s">
-        <v>292</v>
+        <v>231</v>
       </c>
       <c r="E112" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -3976,16 +3976,16 @@
         <v>56</v>
       </c>
       <c r="B113" t="s">
-        <v>231</v>
+        <v>425</v>
       </c>
       <c r="C113" t="s">
-        <v>232</v>
+        <v>403</v>
       </c>
       <c r="D113" t="s">
-        <v>233</v>
+        <v>404</v>
       </c>
       <c r="E113" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -3993,16 +3993,16 @@
         <v>56</v>
       </c>
       <c r="B114" t="s">
-        <v>427</v>
+        <v>291</v>
       </c>
       <c r="C114" t="s">
-        <v>405</v>
+        <v>292</v>
       </c>
       <c r="D114" t="s">
-        <v>406</v>
+        <v>293</v>
       </c>
       <c r="E114" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -4010,16 +4010,16 @@
         <v>56</v>
       </c>
       <c r="B115" t="s">
-        <v>293</v>
+        <v>318</v>
       </c>
       <c r="C115" t="s">
-        <v>294</v>
+        <v>319</v>
       </c>
       <c r="D115" t="s">
-        <v>295</v>
+        <v>320</v>
       </c>
       <c r="E115" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
@@ -4027,16 +4027,16 @@
         <v>56</v>
       </c>
       <c r="B116" t="s">
-        <v>320</v>
+        <v>237</v>
       </c>
       <c r="C116" t="s">
-        <v>321</v>
+        <v>238</v>
       </c>
       <c r="D116" t="s">
-        <v>322</v>
+        <v>414</v>
       </c>
       <c r="E116" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
@@ -4044,16 +4044,16 @@
         <v>56</v>
       </c>
       <c r="B117" t="s">
-        <v>239</v>
+        <v>428</v>
       </c>
       <c r="C117" t="s">
-        <v>240</v>
+        <v>409</v>
       </c>
       <c r="D117" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="E117" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -4061,16 +4061,16 @@
         <v>56</v>
       </c>
       <c r="B118" t="s">
-        <v>430</v>
+        <v>276</v>
       </c>
       <c r="C118" t="s">
-        <v>411</v>
+        <v>277</v>
       </c>
       <c r="D118" t="s">
-        <v>414</v>
+        <v>278</v>
       </c>
       <c r="E118" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
@@ -4078,16 +4078,16 @@
         <v>56</v>
       </c>
       <c r="B119" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C119" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D119" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="E119" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
@@ -4095,16 +4095,16 @@
         <v>56</v>
       </c>
       <c r="B120" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C120" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D120" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E120" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
@@ -4112,16 +4112,16 @@
         <v>56</v>
       </c>
       <c r="B121" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
       <c r="C121" t="s">
-        <v>285</v>
+        <v>273</v>
       </c>
       <c r="D121" t="s">
-        <v>286</v>
+        <v>368</v>
       </c>
       <c r="E121" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
@@ -4135,10 +4135,10 @@
         <v>275</v>
       </c>
       <c r="D122" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E122" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
@@ -4146,16 +4146,16 @@
         <v>56</v>
       </c>
       <c r="B123" t="s">
-        <v>276</v>
+        <v>263</v>
       </c>
       <c r="C123" t="s">
-        <v>277</v>
+        <v>264</v>
       </c>
       <c r="D123" t="s">
-        <v>371</v>
+        <v>417</v>
       </c>
       <c r="E123" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
@@ -4169,10 +4169,10 @@
         <v>266</v>
       </c>
       <c r="D124" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="E124" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
@@ -4186,10 +4186,10 @@
         <v>268</v>
       </c>
       <c r="D125" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E125" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
@@ -4197,16 +4197,16 @@
         <v>56</v>
       </c>
       <c r="B126" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
       <c r="C126" t="s">
-        <v>270</v>
+        <v>286</v>
       </c>
       <c r="D126" t="s">
-        <v>425</v>
+        <v>287</v>
       </c>
       <c r="E126" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
@@ -4214,16 +4214,16 @@
         <v>56</v>
       </c>
       <c r="B127" t="s">
-        <v>287</v>
+        <v>234</v>
       </c>
       <c r="C127" t="s">
-        <v>288</v>
+        <v>235</v>
       </c>
       <c r="D127" t="s">
-        <v>289</v>
+        <v>236</v>
       </c>
       <c r="E127" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
@@ -4231,16 +4231,16 @@
         <v>56</v>
       </c>
       <c r="B128" t="s">
-        <v>236</v>
+        <v>427</v>
       </c>
       <c r="C128" t="s">
-        <v>237</v>
+        <v>407</v>
       </c>
       <c r="D128" t="s">
-        <v>238</v>
+        <v>408</v>
       </c>
       <c r="E128" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
@@ -4248,16 +4248,16 @@
         <v>56</v>
       </c>
       <c r="B129" t="s">
-        <v>429</v>
+        <v>269</v>
       </c>
       <c r="C129" t="s">
-        <v>409</v>
+        <v>270</v>
       </c>
       <c r="D129" t="s">
-        <v>410</v>
+        <v>271</v>
       </c>
       <c r="E129" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
@@ -4265,16 +4265,16 @@
         <v>56</v>
       </c>
       <c r="B130" t="s">
-        <v>271</v>
+        <v>299</v>
       </c>
       <c r="C130" t="s">
-        <v>272</v>
+        <v>300</v>
       </c>
       <c r="D130" t="s">
-        <v>273</v>
+        <v>301</v>
       </c>
       <c r="E130" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
@@ -4282,16 +4282,16 @@
         <v>56</v>
       </c>
       <c r="B131" t="s">
-        <v>301</v>
+        <v>314</v>
       </c>
       <c r="C131" t="s">
-        <v>302</v>
+        <v>400</v>
       </c>
       <c r="D131" t="s">
-        <v>303</v>
+        <v>399</v>
       </c>
       <c r="E131" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
@@ -4299,16 +4299,16 @@
         <v>56</v>
       </c>
       <c r="B132" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="C132" t="s">
-        <v>402</v>
+        <v>312</v>
       </c>
       <c r="D132" t="s">
-        <v>401</v>
+        <v>313</v>
       </c>
       <c r="E132" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
@@ -4316,16 +4316,16 @@
         <v>56</v>
       </c>
       <c r="B133" t="s">
-        <v>313</v>
+        <v>249</v>
       </c>
       <c r="C133" t="s">
-        <v>314</v>
+        <v>250</v>
       </c>
       <c r="D133" t="s">
-        <v>315</v>
+        <v>251</v>
       </c>
       <c r="E133" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
@@ -4333,16 +4333,16 @@
         <v>56</v>
       </c>
       <c r="B134" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
       <c r="C134" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="D134" t="s">
-        <v>253</v>
+        <v>415</v>
       </c>
       <c r="E134" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
@@ -4350,16 +4350,16 @@
         <v>56</v>
       </c>
       <c r="B135" t="s">
-        <v>241</v>
+        <v>429</v>
       </c>
       <c r="C135" t="s">
-        <v>242</v>
+        <v>410</v>
       </c>
       <c r="D135" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="E135" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
@@ -4367,16 +4367,16 @@
         <v>56</v>
       </c>
       <c r="B136" t="s">
-        <v>431</v>
+        <v>308</v>
       </c>
       <c r="C136" t="s">
-        <v>412</v>
+        <v>309</v>
       </c>
       <c r="D136" t="s">
-        <v>415</v>
+        <v>310</v>
       </c>
       <c r="E136" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
@@ -4384,16 +4384,16 @@
         <v>56</v>
       </c>
       <c r="B137" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="C137" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="D137" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="E137" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
@@ -4401,38 +4401,21 @@
         <v>56</v>
       </c>
       <c r="B138" t="s">
-        <v>304</v>
+        <v>397</v>
       </c>
       <c r="C138" t="s">
-        <v>305</v>
+        <v>398</v>
       </c>
       <c r="D138" t="s">
-        <v>306</v>
+        <v>384</v>
       </c>
       <c r="E138" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>56</v>
-      </c>
-      <c r="B139" t="s">
-        <v>399</v>
-      </c>
-      <c r="C139" t="s">
-        <v>400</v>
-      </c>
-      <c r="D139" t="s">
-        <v>386</v>
-      </c>
-      <c r="E139" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A95:E139">
-    <sortCondition ref="C95:C139"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A94:E138">
+    <sortCondition ref="C94:C138"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -4458,33 +4441,33 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>321</v>
+      </c>
+      <c r="B1" t="s">
+        <v>322</v>
+      </c>
+      <c r="C1" t="s">
         <v>323</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>324</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>325</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>326</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>327</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>328</v>
-      </c>
-      <c r="G1" t="s">
-        <v>329</v>
-      </c>
-      <c r="H1" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B2" t="s">
         <v>22</v>
@@ -4499,10 +4482,10 @@
         <v>56</v>
       </c>
       <c r="F2" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="G2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="H2" t="s">
         <v>54</v>

</xml_diff>